<commit_message>
BR reult summary  files with dblf
</commit_message>
<xml_diff>
--- a/clp/results/BR-Original/_summary/br_original_summary.xlsx
+++ b/clp/results/BR-Original/_summary/br_original_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elahi\Desktop\clp\clp\results\BR-Original\_summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFB0B7-2327-4767-A580-61C4D365DD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DB9462-C3A4-4DE9-BE03-8B80EAD56210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>br_class</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t>max_Z1</t>
-  </si>
-  <si>
-    <t>mean_Z2</t>
-  </si>
-  <si>
-    <t>median_Z2</t>
-  </si>
-  <si>
-    <t>std_Z2</t>
-  </si>
-  <si>
-    <t>min_Z2</t>
-  </si>
-  <si>
-    <t>max_Z2</t>
   </si>
   <si>
     <t>mean_Z3</t>
@@ -545,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ33"/>
+  <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="2" sqref="A1:A1048576 B1:B1048576 D1:D1048576"/>
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +542,7 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,28 +657,13 @@
       <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -714,117 +684,102 @@
         <v>0.94901500000000005</v>
       </c>
       <c r="I2" s="1">
+        <v>9.7216900000000006</v>
+      </c>
+      <c r="J2" s="1">
+        <v>9.6881719999999998</v>
+      </c>
+      <c r="K2" s="1">
+        <v>4.243487</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2.2395830000000001</v>
+      </c>
+      <c r="M2" s="1">
+        <v>18.666667</v>
+      </c>
+      <c r="N2" s="1">
+        <v>3.1238999999999999</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2.6696</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2.3092000000000001</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="R2" s="1">
+        <v>10.8659</v>
+      </c>
+      <c r="S2" s="1">
+        <v>7.9317000000000002</v>
+      </c>
+      <c r="T2" s="1">
+        <v>7.1753999999999998</v>
+      </c>
+      <c r="U2" s="1">
+        <v>5.2851999999999997</v>
+      </c>
+      <c r="V2" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>22.7468</v>
+      </c>
+      <c r="X2" s="1">
+        <v>9.7497000000000007</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>9.8803999999999998</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>6.0853000000000002</v>
+      </c>
+      <c r="AA2" s="1">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>9.7216900000000006</v>
-      </c>
-      <c r="O2" s="1">
-        <v>9.6881719999999998</v>
-      </c>
-      <c r="P2" s="1">
-        <v>4.243487</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>2.2395830000000001</v>
-      </c>
-      <c r="R2" s="1">
-        <v>18.666667</v>
-      </c>
-      <c r="S2" s="1">
-        <v>3.1238999999999999</v>
-      </c>
-      <c r="T2" s="1">
-        <v>2.6696</v>
-      </c>
-      <c r="U2" s="1">
-        <v>2.3092000000000001</v>
-      </c>
-      <c r="V2" s="1">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="W2" s="1">
-        <v>10.8659</v>
-      </c>
-      <c r="X2" s="1">
-        <v>7.9317000000000002</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>7.1753999999999998</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>5.2851999999999997</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>5.2999999999999999E-2</v>
-      </c>
       <c r="AB2" s="1">
-        <v>22.7468</v>
+        <v>23.5227</v>
       </c>
       <c r="AC2" s="1">
-        <v>9.7497000000000007</v>
+        <v>31.52</v>
       </c>
       <c r="AD2" s="1">
-        <v>9.8803999999999998</v>
+        <v>24.5</v>
       </c>
       <c r="AE2" s="1">
-        <v>6.0853000000000002</v>
+        <v>23.570399999999999</v>
       </c>
       <c r="AF2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG2" s="1">
-        <v>23.5227</v>
+        <v>125</v>
       </c>
       <c r="AH2" s="1">
-        <v>31.52</v>
+        <v>0.52557200000000004</v>
       </c>
       <c r="AI2" s="1">
-        <v>24.5</v>
+        <v>7.2029999999999997E-2</v>
       </c>
       <c r="AJ2" s="1">
-        <v>23.570399999999999</v>
+        <v>1.8514550000000001</v>
       </c>
       <c r="AK2" s="1">
-        <v>4</v>
+        <v>4.3540000000000002E-3</v>
       </c>
       <c r="AL2" s="1">
-        <v>125</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>0.52557200000000004</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>7.2029999999999997E-2</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>1.8514550000000001</v>
-      </c>
-      <c r="AP2" s="1">
-        <v>4.3540000000000002E-3</v>
-      </c>
-      <c r="AQ2" s="1">
         <v>15.873789</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1">
         <v>100</v>
@@ -845,117 +800,102 @@
         <v>0.94901500000000005</v>
       </c>
       <c r="I3" s="1">
+        <v>10.729194</v>
+      </c>
+      <c r="J3" s="1">
+        <v>10.104775999999999</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4.7519609999999997</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2.2395830000000001</v>
+      </c>
+      <c r="M3" s="1">
+        <v>26.333333</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3.7122000000000002</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2.8914</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2.8656000000000001</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>15.1104</v>
+      </c>
+      <c r="S3" s="1">
+        <v>9.5991</v>
+      </c>
+      <c r="T3" s="1">
+        <v>7.2961</v>
+      </c>
+      <c r="U3" s="1">
+        <v>7.1336000000000004</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.1951</v>
+      </c>
+      <c r="W3" s="1">
+        <v>31.330500000000001</v>
+      </c>
+      <c r="X3" s="1">
+        <v>9.1567000000000007</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>9.0908999999999995</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>6.0857000000000001</v>
+      </c>
+      <c r="AA3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>10.729194</v>
-      </c>
-      <c r="O3" s="1">
-        <v>10.104775999999999</v>
-      </c>
-      <c r="P3" s="1">
-        <v>4.7519609999999997</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>2.2395830000000001</v>
-      </c>
-      <c r="R3" s="1">
-        <v>26.333333</v>
-      </c>
-      <c r="S3" s="1">
-        <v>3.7122000000000002</v>
-      </c>
-      <c r="T3" s="1">
-        <v>2.8914</v>
-      </c>
-      <c r="U3" s="1">
-        <v>2.8656000000000001</v>
-      </c>
-      <c r="V3" s="1">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="W3" s="1">
-        <v>15.1104</v>
-      </c>
-      <c r="X3" s="1">
-        <v>9.5991</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>7.2961</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>7.1336000000000004</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0.1951</v>
-      </c>
       <c r="AB3" s="1">
-        <v>31.330500000000001</v>
+        <v>22.2727</v>
       </c>
       <c r="AC3" s="1">
-        <v>9.1567000000000007</v>
+        <v>34.33</v>
       </c>
       <c r="AD3" s="1">
-        <v>9.0908999999999995</v>
+        <v>28</v>
       </c>
       <c r="AE3" s="1">
-        <v>6.0857000000000001</v>
+        <v>23.625</v>
       </c>
       <c r="AF3" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG3" s="1">
-        <v>22.2727</v>
+        <v>125</v>
       </c>
       <c r="AH3" s="1">
-        <v>34.33</v>
+        <v>0.51635399999999998</v>
       </c>
       <c r="AI3" s="1">
-        <v>28</v>
+        <v>6.1725000000000002E-2</v>
       </c>
       <c r="AJ3" s="1">
-        <v>23.625</v>
+        <v>1.8387929999999999</v>
       </c>
       <c r="AK3" s="1">
-        <v>4</v>
+        <v>4.6620000000000003E-3</v>
       </c>
       <c r="AL3" s="1">
-        <v>125</v>
-      </c>
-      <c r="AM3" s="1">
-        <v>0.51635399999999998</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>6.1725000000000002E-2</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>1.8387929999999999</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>4.6620000000000003E-3</v>
-      </c>
-      <c r="AQ3" s="1">
         <v>15.652310999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>100</v>
@@ -976,117 +916,102 @@
         <v>0.92301100000000003</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>11.660952999999999</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>11.187405999999999</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>4.6307210000000003</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>3.6414680000000001</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>26.445974</v>
       </c>
       <c r="N4" s="1">
-        <v>11.660952999999999</v>
+        <v>5.6604000000000001</v>
       </c>
       <c r="O4" s="1">
-        <v>11.187405999999999</v>
+        <v>5.1405000000000003</v>
       </c>
       <c r="P4" s="1">
-        <v>4.6307210000000003</v>
+        <v>3.5474999999999999</v>
       </c>
       <c r="Q4" s="1">
-        <v>3.6414680000000001</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="R4" s="1">
-        <v>26.445974</v>
+        <v>15.8573</v>
       </c>
       <c r="S4" s="1">
-        <v>5.6604000000000001</v>
+        <v>6.7622999999999998</v>
       </c>
       <c r="T4" s="1">
-        <v>5.1405000000000003</v>
+        <v>6.4245000000000001</v>
       </c>
       <c r="U4" s="1">
-        <v>3.5474999999999999</v>
+        <v>3.3773</v>
       </c>
       <c r="V4" s="1">
-        <v>2.5899999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="W4" s="1">
-        <v>15.8573</v>
+        <v>15.997999999999999</v>
       </c>
       <c r="X4" s="1">
-        <v>6.7622999999999998</v>
+        <v>9.4861000000000004</v>
       </c>
       <c r="Y4" s="1">
-        <v>6.4245000000000001</v>
+        <v>9.3811999999999998</v>
       </c>
       <c r="Z4" s="1">
-        <v>3.3773</v>
+        <v>3.5752999999999999</v>
       </c>
       <c r="AA4" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>3.0228000000000002</v>
       </c>
       <c r="AB4" s="1">
-        <v>15.997999999999999</v>
+        <v>19.284700000000001</v>
       </c>
       <c r="AC4" s="1">
-        <v>9.4861000000000004</v>
+        <v>28.22</v>
       </c>
       <c r="AD4" s="1">
-        <v>9.3811999999999998</v>
+        <v>23</v>
       </c>
       <c r="AE4" s="1">
-        <v>3.5752999999999999</v>
+        <v>17.683900000000001</v>
       </c>
       <c r="AF4" s="1">
-        <v>3.0228000000000002</v>
+        <v>9</v>
       </c>
       <c r="AG4" s="1">
-        <v>19.284700000000001</v>
+        <v>114</v>
       </c>
       <c r="AH4" s="1">
-        <v>28.22</v>
+        <v>0.23580000000000001</v>
       </c>
       <c r="AI4" s="1">
-        <v>23</v>
+        <v>0.11536100000000001</v>
       </c>
       <c r="AJ4" s="1">
-        <v>17.683900000000001</v>
+        <v>0.36754700000000001</v>
       </c>
       <c r="AK4" s="1">
-        <v>9</v>
+        <v>1.9085000000000001E-2</v>
       </c>
       <c r="AL4" s="1">
-        <v>114</v>
-      </c>
-      <c r="AM4" s="1">
-        <v>0.23580000000000001</v>
-      </c>
-      <c r="AN4" s="1">
-        <v>0.11536100000000001</v>
-      </c>
-      <c r="AO4" s="1">
-        <v>0.36754700000000001</v>
-      </c>
-      <c r="AP4" s="1">
-        <v>1.9085000000000001E-2</v>
-      </c>
-      <c r="AQ4" s="1">
         <v>2.415562</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>100</v>
@@ -1107,117 +1032,102 @@
         <v>0.92457599999999995</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>13.347735</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>12.347286</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>5.5641860000000003</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>3.3926539999999998</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>34.342301999999997</v>
       </c>
       <c r="N5" s="1">
-        <v>13.347735</v>
+        <v>6.8776999999999999</v>
       </c>
       <c r="O5" s="1">
-        <v>12.347286</v>
+        <v>5.9901</v>
       </c>
       <c r="P5" s="1">
-        <v>5.5641860000000003</v>
+        <v>4.2173999999999996</v>
       </c>
       <c r="Q5" s="1">
-        <v>3.3926539999999998</v>
+        <v>0.2621</v>
       </c>
       <c r="R5" s="1">
-        <v>34.342301999999997</v>
+        <v>22.158799999999999</v>
       </c>
       <c r="S5" s="1">
-        <v>6.8776999999999999</v>
+        <v>8.1418999999999997</v>
       </c>
       <c r="T5" s="1">
-        <v>5.9901</v>
+        <v>7.4790999999999999</v>
       </c>
       <c r="U5" s="1">
-        <v>4.2173999999999996</v>
+        <v>4.1805000000000003</v>
       </c>
       <c r="V5" s="1">
-        <v>0.2621</v>
+        <v>0.54610000000000003</v>
       </c>
       <c r="W5" s="1">
-        <v>22.158799999999999</v>
+        <v>20.767900000000001</v>
       </c>
       <c r="X5" s="1">
-        <v>8.1418999999999997</v>
+        <v>9.3665000000000003</v>
       </c>
       <c r="Y5" s="1">
-        <v>7.4790999999999999</v>
+        <v>9.3010999999999999</v>
       </c>
       <c r="Z5" s="1">
-        <v>4.1805000000000003</v>
+        <v>3.7465999999999999</v>
       </c>
       <c r="AA5" s="1">
-        <v>0.54610000000000003</v>
+        <v>3.0848</v>
       </c>
       <c r="AB5" s="1">
-        <v>20.767900000000001</v>
+        <v>20.588699999999999</v>
       </c>
       <c r="AC5" s="1">
-        <v>9.3665000000000003</v>
+        <v>31.04</v>
       </c>
       <c r="AD5" s="1">
-        <v>9.3010999999999999</v>
+        <v>27.5</v>
       </c>
       <c r="AE5" s="1">
-        <v>3.7465999999999999</v>
+        <v>16.986599999999999</v>
       </c>
       <c r="AF5" s="1">
-        <v>3.0848</v>
+        <v>9</v>
       </c>
       <c r="AG5" s="1">
-        <v>20.588699999999999</v>
+        <v>117</v>
       </c>
       <c r="AH5" s="1">
-        <v>31.04</v>
+        <v>0.20452500000000001</v>
       </c>
       <c r="AI5" s="1">
-        <v>27.5</v>
+        <v>8.9000999999999997E-2</v>
       </c>
       <c r="AJ5" s="1">
-        <v>16.986599999999999</v>
+        <v>0.34043899999999999</v>
       </c>
       <c r="AK5" s="1">
-        <v>9</v>
+        <v>1.4795000000000001E-2</v>
       </c>
       <c r="AL5" s="1">
-        <v>117</v>
-      </c>
-      <c r="AM5" s="1">
-        <v>0.20452500000000001</v>
-      </c>
-      <c r="AN5" s="1">
-        <v>8.9000999999999997E-2</v>
-      </c>
-      <c r="AO5" s="1">
-        <v>0.34043899999999999</v>
-      </c>
-      <c r="AP5" s="1">
-        <v>1.4795000000000001E-2</v>
-      </c>
-      <c r="AQ5" s="1">
         <v>2.3041160000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1">
         <v>100</v>
@@ -1238,117 +1148,102 @@
         <v>0.87928899999999999</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>12.51225</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>11.680717</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>4.2671000000000001</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>3.8130850000000001</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>27.953523000000001</v>
       </c>
       <c r="N6" s="1">
-        <v>12.51225</v>
+        <v>6.3609</v>
       </c>
       <c r="O6" s="1">
-        <v>11.680717</v>
+        <v>5.8983999999999996</v>
       </c>
       <c r="P6" s="1">
-        <v>4.2671000000000001</v>
+        <v>3.9443999999999999</v>
       </c>
       <c r="Q6" s="1">
-        <v>3.8130850000000001</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="R6" s="1">
-        <v>27.953523000000001</v>
+        <v>20.702200000000001</v>
       </c>
       <c r="S6" s="1">
-        <v>6.3609</v>
+        <v>6.8798000000000004</v>
       </c>
       <c r="T6" s="1">
-        <v>5.8983999999999996</v>
+        <v>6.6755000000000004</v>
       </c>
       <c r="U6" s="1">
-        <v>3.9443999999999999</v>
+        <v>2.6072000000000002</v>
       </c>
       <c r="V6" s="1">
-        <v>2.6599999999999999E-2</v>
+        <v>0.24779999999999999</v>
       </c>
       <c r="W6" s="1">
-        <v>20.702200000000001</v>
+        <v>12.7613</v>
       </c>
       <c r="X6" s="1">
-        <v>6.8798000000000004</v>
+        <v>9.8081999999999994</v>
       </c>
       <c r="Y6" s="1">
-        <v>6.6755000000000004</v>
+        <v>9.2312999999999992</v>
       </c>
       <c r="Z6" s="1">
-        <v>2.6072000000000002</v>
+        <v>2.7564000000000002</v>
       </c>
       <c r="AA6" s="1">
-        <v>0.24779999999999999</v>
+        <v>5.3516000000000004</v>
       </c>
       <c r="AB6" s="1">
-        <v>12.7613</v>
+        <v>19.297699999999999</v>
       </c>
       <c r="AC6" s="1">
-        <v>9.8081999999999994</v>
+        <v>24.9</v>
       </c>
       <c r="AD6" s="1">
-        <v>9.2312999999999992</v>
+        <v>23</v>
       </c>
       <c r="AE6" s="1">
-        <v>2.7564000000000002</v>
+        <v>10.9724</v>
       </c>
       <c r="AF6" s="1">
-        <v>5.3516000000000004</v>
+        <v>9</v>
       </c>
       <c r="AG6" s="1">
-        <v>19.297699999999999</v>
+        <v>60</v>
       </c>
       <c r="AH6" s="1">
-        <v>24.9</v>
+        <v>0.222882</v>
       </c>
       <c r="AI6" s="1">
-        <v>23</v>
+        <v>0.17905399999999999</v>
       </c>
       <c r="AJ6" s="1">
-        <v>10.9724</v>
+        <v>0.206176</v>
       </c>
       <c r="AK6" s="1">
-        <v>9</v>
+        <v>3.7824000000000003E-2</v>
       </c>
       <c r="AL6" s="1">
-        <v>60</v>
-      </c>
-      <c r="AM6" s="1">
-        <v>0.222882</v>
-      </c>
-      <c r="AN6" s="1">
-        <v>0.17905399999999999</v>
-      </c>
-      <c r="AO6" s="1">
-        <v>0.206176</v>
-      </c>
-      <c r="AP6" s="1">
-        <v>3.7824000000000003E-2</v>
-      </c>
-      <c r="AQ6" s="1">
         <v>1.7452259999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>100</v>
@@ -1369,117 +1264,102 @@
         <v>0.87060800000000005</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>13.943360999999999</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>13.456747999999999</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>4.7476419999999999</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>3.9646889999999999</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>26.675508000000001</v>
       </c>
       <c r="N7" s="1">
-        <v>13.943360999999999</v>
+        <v>7.6040999999999999</v>
       </c>
       <c r="O7" s="1">
-        <v>13.456747999999999</v>
+        <v>7.2205000000000004</v>
       </c>
       <c r="P7" s="1">
-        <v>4.7476419999999999</v>
+        <v>4.4561999999999999</v>
       </c>
       <c r="Q7" s="1">
-        <v>3.9646889999999999</v>
+        <v>0.25729999999999997</v>
       </c>
       <c r="R7" s="1">
-        <v>26.675508000000001</v>
+        <v>20.824400000000001</v>
       </c>
       <c r="S7" s="1">
-        <v>7.6040999999999999</v>
+        <v>7.6619999999999999</v>
       </c>
       <c r="T7" s="1">
-        <v>7.2205000000000004</v>
+        <v>7.5735000000000001</v>
       </c>
       <c r="U7" s="1">
-        <v>4.4561999999999999</v>
+        <v>2.8862999999999999</v>
       </c>
       <c r="V7" s="1">
-        <v>0.25729999999999997</v>
+        <v>0.1212</v>
       </c>
       <c r="W7" s="1">
-        <v>20.824400000000001</v>
+        <v>14.0428</v>
       </c>
       <c r="X7" s="1">
-        <v>7.6619999999999999</v>
+        <v>9.5541999999999998</v>
       </c>
       <c r="Y7" s="1">
-        <v>7.5735000000000001</v>
+        <v>9.7065999999999999</v>
       </c>
       <c r="Z7" s="1">
-        <v>2.8862999999999999</v>
+        <v>2.7879999999999998</v>
       </c>
       <c r="AA7" s="1">
-        <v>0.1212</v>
+        <v>3.9883999999999999</v>
       </c>
       <c r="AB7" s="1">
-        <v>14.0428</v>
+        <v>16.688099999999999</v>
       </c>
       <c r="AC7" s="1">
-        <v>9.5541999999999998</v>
+        <v>27.6</v>
       </c>
       <c r="AD7" s="1">
-        <v>9.7065999999999999</v>
+        <v>26</v>
       </c>
       <c r="AE7" s="1">
-        <v>2.7879999999999998</v>
+        <v>11.2967</v>
       </c>
       <c r="AF7" s="1">
-        <v>3.9883999999999999</v>
+        <v>9</v>
       </c>
       <c r="AG7" s="1">
-        <v>16.688099999999999</v>
+        <v>58</v>
       </c>
       <c r="AH7" s="1">
-        <v>27.6</v>
+        <v>0.18088099999999999</v>
       </c>
       <c r="AI7" s="1">
-        <v>26</v>
+        <v>0.13500200000000001</v>
       </c>
       <c r="AJ7" s="1">
-        <v>11.2967</v>
+        <v>0.17733199999999999</v>
       </c>
       <c r="AK7" s="1">
-        <v>9</v>
+        <v>3.3126999999999997E-2</v>
       </c>
       <c r="AL7" s="1">
-        <v>58</v>
-      </c>
-      <c r="AM7" s="1">
-        <v>0.18088099999999999</v>
-      </c>
-      <c r="AN7" s="1">
-        <v>0.13500200000000001</v>
-      </c>
-      <c r="AO7" s="1">
-        <v>0.17733199999999999</v>
-      </c>
-      <c r="AP7" s="1">
-        <v>3.3126999999999997E-2</v>
-      </c>
-      <c r="AQ7" s="1">
         <v>1.5153559999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1">
         <v>100</v>
@@ -1500,117 +1380,102 @@
         <v>0.88708399999999998</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>11.678819000000001</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>11.311057</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>3.8510209999999998</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>4.4572830000000003</v>
       </c>
       <c r="M8" s="1">
-        <v>0</v>
+        <v>23.474867</v>
       </c>
       <c r="N8" s="1">
-        <v>11.678819000000001</v>
+        <v>5.6811999999999996</v>
       </c>
       <c r="O8" s="1">
-        <v>11.311057</v>
+        <v>5.3087999999999997</v>
       </c>
       <c r="P8" s="1">
-        <v>3.8510209999999998</v>
+        <v>3.4129999999999998</v>
       </c>
       <c r="Q8" s="1">
-        <v>4.4572830000000003</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="R8" s="1">
-        <v>23.474867</v>
+        <v>16.5092</v>
       </c>
       <c r="S8" s="1">
-        <v>5.6811999999999996</v>
+        <v>6.4836</v>
       </c>
       <c r="T8" s="1">
-        <v>5.3087999999999997</v>
+        <v>6.2267999999999999</v>
       </c>
       <c r="U8" s="1">
-        <v>3.4129999999999998</v>
+        <v>2.7797999999999998</v>
       </c>
       <c r="V8" s="1">
-        <v>1.2800000000000001E-2</v>
+        <v>0.2828</v>
       </c>
       <c r="W8" s="1">
-        <v>16.5092</v>
+        <v>14.6465</v>
       </c>
       <c r="X8" s="1">
-        <v>6.4836</v>
+        <v>9.7745999999999995</v>
       </c>
       <c r="Y8" s="1">
-        <v>6.2267999999999999</v>
+        <v>9.4799000000000007</v>
       </c>
       <c r="Z8" s="1">
-        <v>2.7797999999999998</v>
+        <v>2.2328000000000001</v>
       </c>
       <c r="AA8" s="1">
-        <v>0.2828</v>
+        <v>4.7359999999999998</v>
       </c>
       <c r="AB8" s="1">
-        <v>14.6465</v>
+        <v>16.106100000000001</v>
       </c>
       <c r="AC8" s="1">
-        <v>9.7745999999999995</v>
+        <v>23.82</v>
       </c>
       <c r="AD8" s="1">
-        <v>9.4799000000000007</v>
+        <v>22.5</v>
       </c>
       <c r="AE8" s="1">
-        <v>2.2328000000000001</v>
+        <v>9.8158999999999992</v>
       </c>
       <c r="AF8" s="1">
-        <v>4.7359999999999998</v>
+        <v>8</v>
       </c>
       <c r="AG8" s="1">
-        <v>16.106100000000001</v>
+        <v>51</v>
       </c>
       <c r="AH8" s="1">
-        <v>23.82</v>
+        <v>0.282277</v>
       </c>
       <c r="AI8" s="1">
-        <v>22.5</v>
+        <v>0.22023899999999999</v>
       </c>
       <c r="AJ8" s="1">
-        <v>9.8158999999999992</v>
+        <v>0.219916</v>
       </c>
       <c r="AK8" s="1">
-        <v>8</v>
+        <v>6.3714999999999994E-2</v>
       </c>
       <c r="AL8" s="1">
-        <v>51</v>
-      </c>
-      <c r="AM8" s="1">
-        <v>0.282277</v>
-      </c>
-      <c r="AN8" s="1">
-        <v>0.22023899999999999</v>
-      </c>
-      <c r="AO8" s="1">
-        <v>0.219916</v>
-      </c>
-      <c r="AP8" s="1">
-        <v>6.3714999999999994E-2</v>
-      </c>
-      <c r="AQ8" s="1">
         <v>1.58304</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
@@ -1631,117 +1496,102 @@
         <v>0.86871799999999999</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>12.453367</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>11.712681</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>4.0797600000000003</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>4.394069</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>23.325212000000001</v>
       </c>
       <c r="N9" s="1">
-        <v>12.453367</v>
+        <v>6.3848000000000003</v>
       </c>
       <c r="O9" s="1">
-        <v>11.712681</v>
+        <v>6.1298000000000004</v>
       </c>
       <c r="P9" s="1">
-        <v>4.0797600000000003</v>
+        <v>3.6551999999999998</v>
       </c>
       <c r="Q9" s="1">
-        <v>4.394069</v>
+        <v>2.01E-2</v>
       </c>
       <c r="R9" s="1">
-        <v>23.325212000000001</v>
+        <v>17.547799999999999</v>
       </c>
       <c r="S9" s="1">
-        <v>6.3848000000000003</v>
+        <v>6.9063999999999997</v>
       </c>
       <c r="T9" s="1">
-        <v>6.1298000000000004</v>
+        <v>6.7024999999999997</v>
       </c>
       <c r="U9" s="1">
-        <v>3.6551999999999998</v>
+        <v>2.9201000000000001</v>
       </c>
       <c r="V9" s="1">
-        <v>2.01E-2</v>
+        <v>0.2828</v>
       </c>
       <c r="W9" s="1">
-        <v>17.547799999999999</v>
+        <v>14.4192</v>
       </c>
       <c r="X9" s="1">
-        <v>6.9063999999999997</v>
+        <v>9.5553000000000008</v>
       </c>
       <c r="Y9" s="1">
-        <v>6.7024999999999997</v>
+        <v>9.2339000000000002</v>
       </c>
       <c r="Z9" s="1">
-        <v>2.9201000000000001</v>
+        <v>2.3058999999999998</v>
       </c>
       <c r="AA9" s="1">
-        <v>0.2828</v>
+        <v>5.1475</v>
       </c>
       <c r="AB9" s="1">
-        <v>14.4192</v>
+        <v>15.4648</v>
       </c>
       <c r="AC9" s="1">
-        <v>9.5553000000000008</v>
+        <v>25.75</v>
       </c>
       <c r="AD9" s="1">
-        <v>9.2339000000000002</v>
+        <v>23.5</v>
       </c>
       <c r="AE9" s="1">
-        <v>2.3058999999999998</v>
+        <v>9.7415000000000003</v>
       </c>
       <c r="AF9" s="1">
-        <v>5.1475</v>
+        <v>12</v>
       </c>
       <c r="AG9" s="1">
-        <v>15.4648</v>
+        <v>54</v>
       </c>
       <c r="AH9" s="1">
-        <v>25.75</v>
+        <v>0.22973399999999999</v>
       </c>
       <c r="AI9" s="1">
-        <v>23.5</v>
+        <v>0.18170700000000001</v>
       </c>
       <c r="AJ9" s="1">
-        <v>9.7415000000000003</v>
+        <v>0.17511299999999999</v>
       </c>
       <c r="AK9" s="1">
-        <v>12</v>
+        <v>4.1001999999999997E-2</v>
       </c>
       <c r="AL9" s="1">
-        <v>54</v>
-      </c>
-      <c r="AM9" s="1">
-        <v>0.22973399999999999</v>
-      </c>
-      <c r="AN9" s="1">
-        <v>0.18170700000000001</v>
-      </c>
-      <c r="AO9" s="1">
-        <v>0.17511299999999999</v>
-      </c>
-      <c r="AP9" s="1">
-        <v>4.1001999999999997E-2</v>
-      </c>
-      <c r="AQ9" s="1">
         <v>1.249398</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
@@ -1762,117 +1612,102 @@
         <v>0.856985</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>12.072404000000001</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>11.805194</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>3.8694289999999998</v>
       </c>
       <c r="L10" s="1">
-        <v>0</v>
+        <v>5.3079910000000003</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>23.963470999999998</v>
       </c>
       <c r="N10" s="1">
-        <v>12.072404000000001</v>
+        <v>5.7680999999999996</v>
       </c>
       <c r="O10" s="1">
-        <v>11.805194</v>
+        <v>5.5975000000000001</v>
       </c>
       <c r="P10" s="1">
-        <v>3.8694289999999998</v>
+        <v>3.3618999999999999</v>
       </c>
       <c r="Q10" s="1">
-        <v>5.3079910000000003</v>
+        <v>0.1565</v>
       </c>
       <c r="R10" s="1">
-        <v>23.963470999999998</v>
+        <v>16.400500000000001</v>
       </c>
       <c r="S10" s="1">
-        <v>5.7680999999999996</v>
+        <v>6.8301999999999996</v>
       </c>
       <c r="T10" s="1">
-        <v>5.5975000000000001</v>
+        <v>6.4580000000000002</v>
       </c>
       <c r="U10" s="1">
-        <v>3.3618999999999999</v>
+        <v>2.6772999999999998</v>
       </c>
       <c r="V10" s="1">
-        <v>0.1565</v>
+        <v>2.1897000000000002</v>
       </c>
       <c r="W10" s="1">
-        <v>16.400500000000001</v>
+        <v>13.5617</v>
       </c>
       <c r="X10" s="1">
-        <v>6.8301999999999996</v>
+        <v>10.248200000000001</v>
       </c>
       <c r="Y10" s="1">
-        <v>6.4580000000000002</v>
+        <v>10.4064</v>
       </c>
       <c r="Z10" s="1">
-        <v>2.6772999999999998</v>
+        <v>2.1214</v>
       </c>
       <c r="AA10" s="1">
-        <v>2.1897000000000002</v>
+        <v>5.5438000000000001</v>
       </c>
       <c r="AB10" s="1">
-        <v>13.5617</v>
+        <v>16.993600000000001</v>
       </c>
       <c r="AC10" s="1">
-        <v>10.248200000000001</v>
+        <v>24.8</v>
       </c>
       <c r="AD10" s="1">
-        <v>10.4064</v>
+        <v>24</v>
       </c>
       <c r="AE10" s="1">
-        <v>2.1214</v>
+        <v>9.9707000000000008</v>
       </c>
       <c r="AF10" s="1">
-        <v>5.5438000000000001</v>
+        <v>9</v>
       </c>
       <c r="AG10" s="1">
-        <v>16.993600000000001</v>
+        <v>64</v>
       </c>
       <c r="AH10" s="1">
-        <v>24.8</v>
+        <v>0.29866599999999999</v>
       </c>
       <c r="AI10" s="1">
-        <v>24</v>
+        <v>0.25348900000000002</v>
       </c>
       <c r="AJ10" s="1">
-        <v>9.9707000000000008</v>
+        <v>0.19218299999999999</v>
       </c>
       <c r="AK10" s="1">
-        <v>9</v>
+        <v>7.1414000000000005E-2</v>
       </c>
       <c r="AL10" s="1">
-        <v>64</v>
-      </c>
-      <c r="AM10" s="1">
-        <v>0.29866599999999999</v>
-      </c>
-      <c r="AN10" s="1">
-        <v>0.25348900000000002</v>
-      </c>
-      <c r="AO10" s="1">
-        <v>0.19218299999999999</v>
-      </c>
-      <c r="AP10" s="1">
-        <v>7.1414000000000005E-2</v>
-      </c>
-      <c r="AQ10" s="1">
         <v>1.2170369999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1">
         <v>100</v>
@@ -1893,117 +1728,102 @@
         <v>0.85453299999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>12.812355</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>12.518967999999999</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>4.5965100000000003</v>
       </c>
       <c r="L11" s="1">
-        <v>0</v>
+        <v>4.4900529999999996</v>
       </c>
       <c r="M11" s="1">
-        <v>0</v>
+        <v>36.555588</v>
       </c>
       <c r="N11" s="1">
-        <v>12.812355</v>
+        <v>6.5429000000000004</v>
       </c>
       <c r="O11" s="1">
-        <v>12.518967999999999</v>
+        <v>6.2164999999999999</v>
       </c>
       <c r="P11" s="1">
-        <v>4.5965100000000003</v>
+        <v>3.9792000000000001</v>
       </c>
       <c r="Q11" s="1">
-        <v>4.4900529999999996</v>
+        <v>0.32790000000000002</v>
       </c>
       <c r="R11" s="1">
-        <v>36.555588</v>
+        <v>27.269500000000001</v>
       </c>
       <c r="S11" s="1">
-        <v>6.5429000000000004</v>
+        <v>7.0918999999999999</v>
       </c>
       <c r="T11" s="1">
-        <v>6.2164999999999999</v>
+        <v>6.8833000000000002</v>
       </c>
       <c r="U11" s="1">
-        <v>3.9792000000000001</v>
+        <v>2.7031000000000001</v>
       </c>
       <c r="V11" s="1">
-        <v>0.32790000000000002</v>
+        <v>1.0327</v>
       </c>
       <c r="W11" s="1">
-        <v>27.269500000000001</v>
+        <v>13.5983</v>
       </c>
       <c r="X11" s="1">
-        <v>7.0918999999999999</v>
+        <v>9.9147999999999996</v>
       </c>
       <c r="Y11" s="1">
-        <v>6.8833000000000002</v>
+        <v>9.7087000000000003</v>
       </c>
       <c r="Z11" s="1">
-        <v>2.7031000000000001</v>
+        <v>2.2480000000000002</v>
       </c>
       <c r="AA11" s="1">
-        <v>1.0327</v>
+        <v>5.6676000000000002</v>
       </c>
       <c r="AB11" s="1">
-        <v>13.5983</v>
+        <v>16.676200000000001</v>
       </c>
       <c r="AC11" s="1">
-        <v>9.9147999999999996</v>
+        <v>26.44</v>
       </c>
       <c r="AD11" s="1">
-        <v>9.7087000000000003</v>
+        <v>24</v>
       </c>
       <c r="AE11" s="1">
-        <v>2.2480000000000002</v>
+        <v>9.9131</v>
       </c>
       <c r="AF11" s="1">
-        <v>5.6676000000000002</v>
+        <v>9</v>
       </c>
       <c r="AG11" s="1">
-        <v>16.676200000000001</v>
+        <v>57</v>
       </c>
       <c r="AH11" s="1">
-        <v>26.44</v>
+        <v>0.23712800000000001</v>
       </c>
       <c r="AI11" s="1">
-        <v>24</v>
+        <v>0.21792</v>
       </c>
       <c r="AJ11" s="1">
-        <v>9.9131</v>
+        <v>0.14923</v>
       </c>
       <c r="AK11" s="1">
-        <v>9</v>
+        <v>4.6608999999999998E-2</v>
       </c>
       <c r="AL11" s="1">
-        <v>57</v>
-      </c>
-      <c r="AM11" s="1">
-        <v>0.23712800000000001</v>
-      </c>
-      <c r="AN11" s="1">
-        <v>0.21792</v>
-      </c>
-      <c r="AO11" s="1">
-        <v>0.14923</v>
-      </c>
-      <c r="AP11" s="1">
-        <v>4.6608999999999998E-2</v>
-      </c>
-      <c r="AQ11" s="1">
         <v>1.004432</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>100</v>
@@ -2024,117 +1844,102 @@
         <v>0.87504199999999999</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>11.404648</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>11.518046</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>2.674328</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>5.5467190000000004</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>18.706264999999998</v>
       </c>
       <c r="N12" s="1">
-        <v>11.404648</v>
+        <v>5.3691000000000004</v>
       </c>
       <c r="O12" s="1">
-        <v>11.518046</v>
+        <v>5.3606999999999996</v>
       </c>
       <c r="P12" s="1">
-        <v>2.674328</v>
+        <v>2.4136000000000002</v>
       </c>
       <c r="Q12" s="1">
-        <v>5.5467190000000004</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="R12" s="1">
-        <v>18.706264999999998</v>
+        <v>11.8733</v>
       </c>
       <c r="S12" s="1">
-        <v>5.3691000000000004</v>
+        <v>6.0692000000000004</v>
       </c>
       <c r="T12" s="1">
-        <v>5.3606999999999996</v>
+        <v>6.1898999999999997</v>
       </c>
       <c r="U12" s="1">
-        <v>2.4136000000000002</v>
+        <v>2.0968</v>
       </c>
       <c r="V12" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.0331999999999999</v>
       </c>
       <c r="W12" s="1">
-        <v>11.8733</v>
+        <v>10.5837</v>
       </c>
       <c r="X12" s="1">
-        <v>6.0692000000000004</v>
+        <v>10.301399999999999</v>
       </c>
       <c r="Y12" s="1">
-        <v>6.1898999999999997</v>
+        <v>10.1076</v>
       </c>
       <c r="Z12" s="1">
-        <v>2.0968</v>
+        <v>2.0388000000000002</v>
       </c>
       <c r="AA12" s="1">
-        <v>1.0331999999999999</v>
+        <v>5.8879000000000001</v>
       </c>
       <c r="AB12" s="1">
-        <v>10.5837</v>
+        <v>15.0923</v>
       </c>
       <c r="AC12" s="1">
-        <v>10.301399999999999</v>
+        <v>24.33</v>
       </c>
       <c r="AD12" s="1">
-        <v>10.1076</v>
+        <v>22.5</v>
       </c>
       <c r="AE12" s="1">
-        <v>2.0388000000000002</v>
+        <v>8.1016999999999992</v>
       </c>
       <c r="AF12" s="1">
-        <v>5.8879000000000001</v>
+        <v>10</v>
       </c>
       <c r="AG12" s="1">
-        <v>15.0923</v>
+        <v>52</v>
       </c>
       <c r="AH12" s="1">
-        <v>24.33</v>
+        <v>0.32333200000000001</v>
       </c>
       <c r="AI12" s="1">
-        <v>22.5</v>
+        <v>0.27456599999999998</v>
       </c>
       <c r="AJ12" s="1">
-        <v>8.1016999999999992</v>
+        <v>0.199071</v>
       </c>
       <c r="AK12" s="1">
-        <v>10</v>
+        <v>9.4571000000000002E-2</v>
       </c>
       <c r="AL12" s="1">
-        <v>52</v>
-      </c>
-      <c r="AM12" s="1">
-        <v>0.32333200000000001</v>
-      </c>
-      <c r="AN12" s="1">
-        <v>0.27456599999999998</v>
-      </c>
-      <c r="AO12" s="1">
-        <v>0.199071</v>
-      </c>
-      <c r="AP12" s="1">
-        <v>9.4571000000000002E-2</v>
-      </c>
-      <c r="AQ12" s="1">
         <v>1.085658</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <v>100</v>
@@ -2155,117 +1960,102 @@
         <v>0.86448800000000003</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>12.548774999999999</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
+        <v>12.079404</v>
       </c>
       <c r="K13" s="1">
-        <v>0</v>
+        <v>3.425014</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>6.4668289999999997</v>
       </c>
       <c r="M13" s="1">
-        <v>0</v>
+        <v>22.156860999999999</v>
       </c>
       <c r="N13" s="1">
-        <v>12.548774999999999</v>
+        <v>6.3201000000000001</v>
       </c>
       <c r="O13" s="1">
-        <v>12.079404</v>
+        <v>6.3497000000000003</v>
       </c>
       <c r="P13" s="1">
-        <v>3.425014</v>
+        <v>3.0268000000000002</v>
       </c>
       <c r="Q13" s="1">
-        <v>6.4668289999999997</v>
+        <v>0.25950000000000001</v>
       </c>
       <c r="R13" s="1">
-        <v>22.156860999999999</v>
+        <v>14.410500000000001</v>
       </c>
       <c r="S13" s="1">
-        <v>6.3201000000000001</v>
+        <v>6.7496999999999998</v>
       </c>
       <c r="T13" s="1">
-        <v>6.3497000000000003</v>
+        <v>6.5955000000000004</v>
       </c>
       <c r="U13" s="1">
-        <v>3.0268000000000002</v>
+        <v>2.5979000000000001</v>
       </c>
       <c r="V13" s="1">
-        <v>0.25950000000000001</v>
+        <v>0.47960000000000003</v>
       </c>
       <c r="W13" s="1">
-        <v>14.410500000000001</v>
+        <v>13.187900000000001</v>
       </c>
       <c r="X13" s="1">
-        <v>6.7496999999999998</v>
+        <v>10.1547</v>
       </c>
       <c r="Y13" s="1">
-        <v>6.5955000000000004</v>
+        <v>9.7698</v>
       </c>
       <c r="Z13" s="1">
-        <v>2.5979000000000001</v>
+        <v>2.4089999999999998</v>
       </c>
       <c r="AA13" s="1">
-        <v>0.47960000000000003</v>
+        <v>4.4489000000000001</v>
       </c>
       <c r="AB13" s="1">
-        <v>13.187900000000001</v>
+        <v>15.3725</v>
       </c>
       <c r="AC13" s="1">
-        <v>10.1547</v>
+        <v>27.02</v>
       </c>
       <c r="AD13" s="1">
-        <v>9.7698</v>
+        <v>26</v>
       </c>
       <c r="AE13" s="1">
-        <v>2.4089999999999998</v>
+        <v>8.8476999999999997</v>
       </c>
       <c r="AF13" s="1">
-        <v>4.4489000000000001</v>
+        <v>13</v>
       </c>
       <c r="AG13" s="1">
-        <v>15.3725</v>
+        <v>58</v>
       </c>
       <c r="AH13" s="1">
-        <v>27.02</v>
+        <v>0.25157299999999999</v>
       </c>
       <c r="AI13" s="1">
-        <v>26</v>
+        <v>0.22284899999999999</v>
       </c>
       <c r="AJ13" s="1">
-        <v>8.8476999999999997</v>
+        <v>0.146205</v>
       </c>
       <c r="AK13" s="1">
-        <v>13</v>
+        <v>8.0376000000000003E-2</v>
       </c>
       <c r="AL13" s="1">
-        <v>58</v>
-      </c>
-      <c r="AM13" s="1">
-        <v>0.25157299999999999</v>
-      </c>
-      <c r="AN13" s="1">
-        <v>0.22284899999999999</v>
-      </c>
-      <c r="AO13" s="1">
-        <v>0.146205</v>
-      </c>
-      <c r="AP13" s="1">
-        <v>8.0376000000000003E-2</v>
-      </c>
-      <c r="AQ13" s="1">
         <v>0.91560799999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1">
         <v>100</v>
@@ -2286,117 +2076,102 @@
         <v>0.83479899999999996</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>11.845431</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>11.432444</v>
       </c>
       <c r="K14" s="1">
-        <v>0</v>
+        <v>3.2320669999999998</v>
       </c>
       <c r="L14" s="1">
-        <v>0</v>
+        <v>6.7762510000000002</v>
       </c>
       <c r="M14" s="1">
-        <v>0</v>
+        <v>23.489439000000001</v>
       </c>
       <c r="N14" s="1">
-        <v>11.845431</v>
+        <v>5.5937000000000001</v>
       </c>
       <c r="O14" s="1">
-        <v>11.432444</v>
+        <v>5.2347999999999999</v>
       </c>
       <c r="P14" s="1">
-        <v>3.2320669999999998</v>
+        <v>3.0560999999999998</v>
       </c>
       <c r="Q14" s="1">
-        <v>6.7762510000000002</v>
+        <v>1.0333000000000001</v>
       </c>
       <c r="R14" s="1">
-        <v>23.489439000000001</v>
+        <v>17.715</v>
       </c>
       <c r="S14" s="1">
-        <v>5.5937000000000001</v>
+        <v>6.3628999999999998</v>
       </c>
       <c r="T14" s="1">
-        <v>5.2347999999999999</v>
+        <v>6.7130999999999998</v>
       </c>
       <c r="U14" s="1">
-        <v>3.0560999999999998</v>
+        <v>2.1999</v>
       </c>
       <c r="V14" s="1">
-        <v>1.0333000000000001</v>
+        <v>0.74029999999999996</v>
       </c>
       <c r="W14" s="1">
-        <v>17.715</v>
+        <v>10.9369</v>
       </c>
       <c r="X14" s="1">
-        <v>6.3628999999999998</v>
+        <v>10.5909</v>
       </c>
       <c r="Y14" s="1">
-        <v>6.7130999999999998</v>
+        <v>10.7286</v>
       </c>
       <c r="Z14" s="1">
-        <v>2.1999</v>
+        <v>1.7778</v>
       </c>
       <c r="AA14" s="1">
-        <v>0.74029999999999996</v>
+        <v>6.2465999999999999</v>
       </c>
       <c r="AB14" s="1">
-        <v>10.9369</v>
+        <v>14.8894</v>
       </c>
       <c r="AC14" s="1">
-        <v>10.5909</v>
+        <v>24.48</v>
       </c>
       <c r="AD14" s="1">
-        <v>10.7286</v>
+        <v>23.5</v>
       </c>
       <c r="AE14" s="1">
-        <v>1.7778</v>
+        <v>7.5498000000000003</v>
       </c>
       <c r="AF14" s="1">
-        <v>6.2465999999999999</v>
+        <v>10</v>
       </c>
       <c r="AG14" s="1">
-        <v>14.8894</v>
+        <v>49</v>
       </c>
       <c r="AH14" s="1">
-        <v>24.48</v>
+        <v>0.33202500000000001</v>
       </c>
       <c r="AI14" s="1">
-        <v>23.5</v>
+        <v>0.31012099999999998</v>
       </c>
       <c r="AJ14" s="1">
-        <v>7.5498000000000003</v>
+        <v>0.15551200000000001</v>
       </c>
       <c r="AK14" s="1">
-        <v>10</v>
+        <v>7.9534999999999995E-2</v>
       </c>
       <c r="AL14" s="1">
-        <v>49</v>
-      </c>
-      <c r="AM14" s="1">
-        <v>0.33202500000000001</v>
-      </c>
-      <c r="AN14" s="1">
-        <v>0.31012099999999998</v>
-      </c>
-      <c r="AO14" s="1">
-        <v>0.15551200000000001</v>
-      </c>
-      <c r="AP14" s="1">
-        <v>7.9534999999999995E-2</v>
-      </c>
-      <c r="AQ14" s="1">
         <v>0.99646100000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -2417,117 +2192,102 @@
         <v>0.824376</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>12.784575999999999</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>12.222923</v>
       </c>
       <c r="K15" s="1">
-        <v>0</v>
+        <v>3.5072760000000001</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>6.4747430000000001</v>
       </c>
       <c r="M15" s="1">
-        <v>0</v>
+        <v>22.331357000000001</v>
       </c>
       <c r="N15" s="1">
-        <v>12.784575999999999</v>
+        <v>6.2089999999999996</v>
       </c>
       <c r="O15" s="1">
-        <v>12.222923</v>
+        <v>6.0815000000000001</v>
       </c>
       <c r="P15" s="1">
-        <v>3.5072760000000001</v>
+        <v>3.0760000000000001</v>
       </c>
       <c r="Q15" s="1">
-        <v>6.4747430000000001</v>
+        <v>9.7900000000000001E-2</v>
       </c>
       <c r="R15" s="1">
-        <v>22.331357000000001</v>
+        <v>16.155799999999999</v>
       </c>
       <c r="S15" s="1">
-        <v>6.2089999999999996</v>
+        <v>7.4165000000000001</v>
       </c>
       <c r="T15" s="1">
-        <v>6.0815000000000001</v>
+        <v>7.3634000000000004</v>
       </c>
       <c r="U15" s="1">
-        <v>3.0760000000000001</v>
+        <v>2.7642000000000002</v>
       </c>
       <c r="V15" s="1">
-        <v>9.7900000000000001E-2</v>
+        <v>1.3642000000000001</v>
       </c>
       <c r="W15" s="1">
-        <v>16.155799999999999</v>
+        <v>14.822699999999999</v>
       </c>
       <c r="X15" s="1">
-        <v>7.4165000000000001</v>
+        <v>10.388999999999999</v>
       </c>
       <c r="Y15" s="1">
-        <v>7.3634000000000004</v>
+        <v>10.1555</v>
       </c>
       <c r="Z15" s="1">
-        <v>2.7642000000000002</v>
+        <v>2.0261999999999998</v>
       </c>
       <c r="AA15" s="1">
-        <v>1.3642000000000001</v>
+        <v>6.5598999999999998</v>
       </c>
       <c r="AB15" s="1">
-        <v>14.822699999999999</v>
+        <v>16.156300000000002</v>
       </c>
       <c r="AC15" s="1">
-        <v>10.388999999999999</v>
+        <v>26.53</v>
       </c>
       <c r="AD15" s="1">
-        <v>10.1555</v>
+        <v>26</v>
       </c>
       <c r="AE15" s="1">
-        <v>2.0261999999999998</v>
+        <v>7.4946999999999999</v>
       </c>
       <c r="AF15" s="1">
-        <v>6.5598999999999998</v>
+        <v>13</v>
       </c>
       <c r="AG15" s="1">
-        <v>16.156300000000002</v>
+        <v>50</v>
       </c>
       <c r="AH15" s="1">
-        <v>26.53</v>
+        <v>0.253164</v>
       </c>
       <c r="AI15" s="1">
-        <v>26</v>
+        <v>0.24147199999999999</v>
       </c>
       <c r="AJ15" s="1">
-        <v>7.4946999999999999</v>
+        <v>0.1137</v>
       </c>
       <c r="AK15" s="1">
-        <v>13</v>
+        <v>8.1331000000000001E-2</v>
       </c>
       <c r="AL15" s="1">
-        <v>50</v>
-      </c>
-      <c r="AM15" s="1">
-        <v>0.253164</v>
-      </c>
-      <c r="AN15" s="1">
-        <v>0.24147199999999999</v>
-      </c>
-      <c r="AO15" s="1">
-        <v>0.1137</v>
-      </c>
-      <c r="AP15" s="1">
-        <v>8.1331000000000001E-2</v>
-      </c>
-      <c r="AQ15" s="1">
         <v>0.69569499999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1">
         <v>100</v>
@@ -2548,117 +2308,102 @@
         <v>0.83341100000000001</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>11.743327000000001</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>11.563437</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>3.1335809999999999</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>5.0646779999999998</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>19.405633000000002</v>
       </c>
       <c r="N16" s="1">
-        <v>11.743327000000001</v>
+        <v>5.1683000000000003</v>
       </c>
       <c r="O16" s="1">
-        <v>11.563437</v>
+        <v>5.0692000000000004</v>
       </c>
       <c r="P16" s="1">
-        <v>3.1335809999999999</v>
+        <v>2.8458999999999999</v>
       </c>
       <c r="Q16" s="1">
-        <v>5.0646779999999998</v>
+        <v>0.23880000000000001</v>
       </c>
       <c r="R16" s="1">
-        <v>19.405633000000002</v>
+        <v>11.7401</v>
       </c>
       <c r="S16" s="1">
-        <v>5.1683000000000003</v>
+        <v>6.6576000000000004</v>
       </c>
       <c r="T16" s="1">
-        <v>5.0692000000000004</v>
+        <v>6.6733000000000002</v>
       </c>
       <c r="U16" s="1">
-        <v>2.8458999999999999</v>
+        <v>2.2210000000000001</v>
       </c>
       <c r="V16" s="1">
-        <v>0.23880000000000001</v>
+        <v>0.84130000000000005</v>
       </c>
       <c r="W16" s="1">
-        <v>11.7401</v>
+        <v>11.557</v>
       </c>
       <c r="X16" s="1">
-        <v>6.6576000000000004</v>
+        <v>11.1394</v>
       </c>
       <c r="Y16" s="1">
-        <v>6.6733000000000002</v>
+        <v>11.0688</v>
       </c>
       <c r="Z16" s="1">
-        <v>2.2210000000000001</v>
+        <v>1.9781</v>
       </c>
       <c r="AA16" s="1">
-        <v>0.84130000000000005</v>
+        <v>6.2686999999999999</v>
       </c>
       <c r="AB16" s="1">
-        <v>11.557</v>
+        <v>15.9725</v>
       </c>
       <c r="AC16" s="1">
-        <v>11.1394</v>
+        <v>25.5</v>
       </c>
       <c r="AD16" s="1">
-        <v>11.0688</v>
+        <v>25</v>
       </c>
       <c r="AE16" s="1">
-        <v>1.9781</v>
+        <v>6.9957000000000003</v>
       </c>
       <c r="AF16" s="1">
-        <v>6.2686999999999999</v>
+        <v>10</v>
       </c>
       <c r="AG16" s="1">
-        <v>15.9725</v>
+        <v>46</v>
       </c>
       <c r="AH16" s="1">
-        <v>25.5</v>
+        <v>0.34978199999999998</v>
       </c>
       <c r="AI16" s="1">
-        <v>25</v>
+        <v>0.32252700000000001</v>
       </c>
       <c r="AJ16" s="1">
-        <v>6.9957000000000003</v>
+        <v>0.158418</v>
       </c>
       <c r="AK16" s="1">
-        <v>10</v>
+        <v>0.102882</v>
       </c>
       <c r="AL16" s="1">
-        <v>46</v>
-      </c>
-      <c r="AM16" s="1">
-        <v>0.34978199999999998</v>
-      </c>
-      <c r="AN16" s="1">
-        <v>0.32252700000000001</v>
-      </c>
-      <c r="AO16" s="1">
-        <v>0.158418</v>
-      </c>
-      <c r="AP16" s="1">
-        <v>0.102882</v>
-      </c>
-      <c r="AQ16" s="1">
         <v>0.79335500000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1">
         <v>100</v>
@@ -2679,117 +2424,102 @@
         <v>0.80957599999999996</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>13.107362</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>13.008385000000001</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>3.353612</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>6.9281259999999998</v>
       </c>
       <c r="M17" s="1">
-        <v>0</v>
+        <v>22.275659000000001</v>
       </c>
       <c r="N17" s="1">
-        <v>13.107362</v>
+        <v>6.4905999999999997</v>
       </c>
       <c r="O17" s="1">
-        <v>13.008385000000001</v>
+        <v>6.2226999999999997</v>
       </c>
       <c r="P17" s="1">
-        <v>3.353612</v>
+        <v>3.2603</v>
       </c>
       <c r="Q17" s="1">
-        <v>6.9281259999999998</v>
+        <v>0.94630000000000003</v>
       </c>
       <c r="R17" s="1">
-        <v>22.275659000000001</v>
+        <v>16.334700000000002</v>
       </c>
       <c r="S17" s="1">
-        <v>6.4905999999999997</v>
+        <v>7.0201000000000002</v>
       </c>
       <c r="T17" s="1">
-        <v>6.2226999999999997</v>
+        <v>7.1158000000000001</v>
       </c>
       <c r="U17" s="1">
-        <v>3.2603</v>
+        <v>2.5141</v>
       </c>
       <c r="V17" s="1">
-        <v>0.94630000000000003</v>
+        <v>0.33610000000000001</v>
       </c>
       <c r="W17" s="1">
-        <v>16.334700000000002</v>
+        <v>14.595599999999999</v>
       </c>
       <c r="X17" s="1">
-        <v>7.0201000000000002</v>
+        <v>10.9353</v>
       </c>
       <c r="Y17" s="1">
-        <v>7.1158000000000001</v>
+        <v>10.906700000000001</v>
       </c>
       <c r="Z17" s="1">
-        <v>2.5141</v>
+        <v>2.0527000000000002</v>
       </c>
       <c r="AA17" s="1">
-        <v>0.33610000000000001</v>
+        <v>4.5233999999999996</v>
       </c>
       <c r="AB17" s="1">
-        <v>14.595599999999999</v>
+        <v>16.8841</v>
       </c>
       <c r="AC17" s="1">
-        <v>10.9353</v>
+        <v>28.47</v>
       </c>
       <c r="AD17" s="1">
-        <v>10.906700000000001</v>
+        <v>28</v>
       </c>
       <c r="AE17" s="1">
-        <v>2.0527000000000002</v>
+        <v>6.4690000000000003</v>
       </c>
       <c r="AF17" s="1">
-        <v>4.5233999999999996</v>
+        <v>12</v>
       </c>
       <c r="AG17" s="1">
-        <v>16.8841</v>
+        <v>44</v>
       </c>
       <c r="AH17" s="1">
-        <v>28.47</v>
+        <v>0.25806899999999999</v>
       </c>
       <c r="AI17" s="1">
-        <v>28</v>
+        <v>0.239395</v>
       </c>
       <c r="AJ17" s="1">
-        <v>6.4690000000000003</v>
+        <v>0.109685</v>
       </c>
       <c r="AK17" s="1">
-        <v>12</v>
+        <v>9.2744999999999994E-2</v>
       </c>
       <c r="AL17" s="1">
-        <v>44</v>
-      </c>
-      <c r="AM17" s="1">
-        <v>0.25806899999999999</v>
-      </c>
-      <c r="AN17" s="1">
-        <v>0.239395</v>
-      </c>
-      <c r="AO17" s="1">
-        <v>0.109685</v>
-      </c>
-      <c r="AP17" s="1">
-        <v>9.2744999999999994E-2</v>
-      </c>
-      <c r="AQ17" s="1">
         <v>0.63460499999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1">
         <v>100</v>
@@ -2810,117 +2540,102 @@
         <v>0.79290799999999995</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>11.003265000000001</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>10.6142</v>
       </c>
       <c r="K18" s="1">
-        <v>0</v>
+        <v>2.4090090000000002</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>6.1984069999999996</v>
       </c>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>19.494297</v>
       </c>
       <c r="N18" s="1">
-        <v>11.003265000000001</v>
+        <v>4.5814000000000004</v>
       </c>
       <c r="O18" s="1">
-        <v>10.6142</v>
+        <v>4.4267000000000003</v>
       </c>
       <c r="P18" s="1">
-        <v>2.4090090000000002</v>
+        <v>2.1179999999999999</v>
       </c>
       <c r="Q18" s="1">
-        <v>6.1984069999999996</v>
+        <v>0.13109999999999999</v>
       </c>
       <c r="R18" s="1">
-        <v>19.494297</v>
+        <v>10.527900000000001</v>
       </c>
       <c r="S18" s="1">
-        <v>4.5814000000000004</v>
+        <v>6.0324999999999998</v>
       </c>
       <c r="T18" s="1">
-        <v>4.4267000000000003</v>
+        <v>6.0077999999999996</v>
       </c>
       <c r="U18" s="1">
-        <v>2.1179999999999999</v>
+        <v>2.1427</v>
       </c>
       <c r="V18" s="1">
-        <v>0.13109999999999999</v>
+        <v>1.6321000000000001</v>
       </c>
       <c r="W18" s="1">
-        <v>10.527900000000001</v>
+        <v>12.4154</v>
       </c>
       <c r="X18" s="1">
-        <v>6.0324999999999998</v>
+        <v>11.3543</v>
       </c>
       <c r="Y18" s="1">
-        <v>6.0077999999999996</v>
+        <v>11.0482</v>
       </c>
       <c r="Z18" s="1">
-        <v>2.1427</v>
+        <v>1.9776</v>
       </c>
       <c r="AA18" s="1">
-        <v>1.6321000000000001</v>
+        <v>7.3219000000000003</v>
       </c>
       <c r="AB18" s="1">
-        <v>12.4154</v>
+        <v>17.948699999999999</v>
       </c>
       <c r="AC18" s="1">
-        <v>11.3543</v>
+        <v>27.39</v>
       </c>
       <c r="AD18" s="1">
-        <v>11.0482</v>
+        <v>27</v>
       </c>
       <c r="AE18" s="1">
-        <v>1.9776</v>
+        <v>6.8562000000000003</v>
       </c>
       <c r="AF18" s="1">
-        <v>7.3219000000000003</v>
+        <v>13</v>
       </c>
       <c r="AG18" s="1">
-        <v>17.948699999999999</v>
+        <v>53</v>
       </c>
       <c r="AH18" s="1">
-        <v>27.39</v>
+        <v>0.36780299999999999</v>
       </c>
       <c r="AI18" s="1">
-        <v>27</v>
+        <v>0.35758400000000001</v>
       </c>
       <c r="AJ18" s="1">
-        <v>6.8562000000000003</v>
+        <v>0.13760600000000001</v>
       </c>
       <c r="AK18" s="1">
-        <v>13</v>
+        <v>0.118368</v>
       </c>
       <c r="AL18" s="1">
-        <v>53</v>
-      </c>
-      <c r="AM18" s="1">
-        <v>0.36780299999999999</v>
-      </c>
-      <c r="AN18" s="1">
-        <v>0.35758400000000001</v>
-      </c>
-      <c r="AO18" s="1">
-        <v>0.13760600000000001</v>
-      </c>
-      <c r="AP18" s="1">
-        <v>0.118368</v>
-      </c>
-      <c r="AQ18" s="1">
         <v>0.75657399999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1">
         <v>100</v>
@@ -2941,117 +2656,102 @@
         <v>0.77444900000000005</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>11.932839</v>
       </c>
       <c r="J19" s="1">
-        <v>0</v>
+        <v>10.993589999999999</v>
       </c>
       <c r="K19" s="1">
-        <v>0</v>
+        <v>4.1564230000000002</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>6.0054780000000001</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>30.78359</v>
       </c>
       <c r="N19" s="1">
-        <v>11.932839</v>
+        <v>5.2282999999999999</v>
       </c>
       <c r="O19" s="1">
-        <v>10.993589999999999</v>
+        <v>4.9595000000000002</v>
       </c>
       <c r="P19" s="1">
-        <v>4.1564230000000002</v>
+        <v>3.7576000000000001</v>
       </c>
       <c r="Q19" s="1">
-        <v>6.0054780000000001</v>
+        <v>0.28129999999999999</v>
       </c>
       <c r="R19" s="1">
-        <v>30.78359</v>
+        <v>22.321100000000001</v>
       </c>
       <c r="S19" s="1">
-        <v>5.2282999999999999</v>
+        <v>6.8216999999999999</v>
       </c>
       <c r="T19" s="1">
-        <v>4.9595000000000002</v>
+        <v>6.4962</v>
       </c>
       <c r="U19" s="1">
-        <v>3.7576000000000001</v>
+        <v>2.5030999999999999</v>
       </c>
       <c r="V19" s="1">
-        <v>0.28129999999999999</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="W19" s="1">
-        <v>22.321100000000001</v>
+        <v>13.117699999999999</v>
       </c>
       <c r="X19" s="1">
-        <v>6.8216999999999999</v>
+        <v>11.3216</v>
       </c>
       <c r="Y19" s="1">
-        <v>6.4962</v>
+        <v>10.972300000000001</v>
       </c>
       <c r="Z19" s="1">
-        <v>2.5030999999999999</v>
+        <v>1.8344</v>
       </c>
       <c r="AA19" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>7.6215999999999999</v>
       </c>
       <c r="AB19" s="1">
-        <v>13.117699999999999</v>
+        <v>16.990600000000001</v>
       </c>
       <c r="AC19" s="1">
-        <v>11.3216</v>
+        <v>30.03</v>
       </c>
       <c r="AD19" s="1">
-        <v>10.972300000000001</v>
+        <v>30</v>
       </c>
       <c r="AE19" s="1">
-        <v>1.8344</v>
+        <v>6.274</v>
       </c>
       <c r="AF19" s="1">
-        <v>7.6215999999999999</v>
+        <v>16</v>
       </c>
       <c r="AG19" s="1">
-        <v>16.990600000000001</v>
+        <v>52</v>
       </c>
       <c r="AH19" s="1">
-        <v>30.03</v>
+        <v>0.27580500000000002</v>
       </c>
       <c r="AI19" s="1">
-        <v>30</v>
+        <v>0.26247900000000002</v>
       </c>
       <c r="AJ19" s="1">
-        <v>6.274</v>
+        <v>9.2519000000000004E-2</v>
       </c>
       <c r="AK19" s="1">
-        <v>16</v>
+        <v>0.10778699999999999</v>
       </c>
       <c r="AL19" s="1">
-        <v>52</v>
-      </c>
-      <c r="AM19" s="1">
-        <v>0.27580500000000002</v>
-      </c>
-      <c r="AN19" s="1">
-        <v>0.26247900000000002</v>
-      </c>
-      <c r="AO19" s="1">
-        <v>9.2519000000000004E-2</v>
-      </c>
-      <c r="AP19" s="1">
-        <v>0.10778699999999999</v>
-      </c>
-      <c r="AQ19" s="1">
         <v>0.60431000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1">
         <v>100</v>
@@ -3072,117 +2772,102 @@
         <v>0.79935199999999995</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>10.417897</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>10.130627</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>2.6157159999999999</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>5.5387219999999999</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>19.705573999999999</v>
       </c>
       <c r="N20" s="1">
-        <v>10.417897</v>
+        <v>4.1638999999999999</v>
       </c>
       <c r="O20" s="1">
-        <v>10.130627</v>
+        <v>3.8403</v>
       </c>
       <c r="P20" s="1">
-        <v>2.6157159999999999</v>
+        <v>2.3128000000000002</v>
       </c>
       <c r="Q20" s="1">
-        <v>5.5387219999999999</v>
+        <v>0.42230000000000001</v>
       </c>
       <c r="R20" s="1">
-        <v>19.705573999999999</v>
+        <v>11.085800000000001</v>
       </c>
       <c r="S20" s="1">
-        <v>4.1638999999999999</v>
+        <v>5.5998999999999999</v>
       </c>
       <c r="T20" s="1">
-        <v>3.8403</v>
+        <v>5.6234000000000002</v>
       </c>
       <c r="U20" s="1">
-        <v>2.3128000000000002</v>
+        <v>2.4262000000000001</v>
       </c>
       <c r="V20" s="1">
-        <v>0.42230000000000001</v>
+        <v>7.2700000000000001E-2</v>
       </c>
       <c r="W20" s="1">
-        <v>11.085800000000001</v>
+        <v>12.640599999999999</v>
       </c>
       <c r="X20" s="1">
-        <v>5.5998999999999999</v>
+        <v>11.333600000000001</v>
       </c>
       <c r="Y20" s="1">
-        <v>5.6234000000000002</v>
+        <v>11.533899999999999</v>
       </c>
       <c r="Z20" s="1">
-        <v>2.4262000000000001</v>
+        <v>1.5527</v>
       </c>
       <c r="AA20" s="1">
-        <v>7.2700000000000001E-2</v>
+        <v>8.3544999999999998</v>
       </c>
       <c r="AB20" s="1">
-        <v>12.640599999999999</v>
+        <v>15.626300000000001</v>
       </c>
       <c r="AC20" s="1">
-        <v>11.333600000000001</v>
+        <v>27.38</v>
       </c>
       <c r="AD20" s="1">
-        <v>11.533899999999999</v>
+        <v>26.5</v>
       </c>
       <c r="AE20" s="1">
-        <v>1.5527</v>
+        <v>6.2389999999999999</v>
       </c>
       <c r="AF20" s="1">
-        <v>8.3544999999999998</v>
+        <v>13</v>
       </c>
       <c r="AG20" s="1">
-        <v>15.626300000000001</v>
+        <v>43</v>
       </c>
       <c r="AH20" s="1">
-        <v>27.38</v>
+        <v>0.36592400000000003</v>
       </c>
       <c r="AI20" s="1">
-        <v>26.5</v>
+        <v>0.337231</v>
       </c>
       <c r="AJ20" s="1">
-        <v>6.2389999999999999</v>
+        <v>0.122171</v>
       </c>
       <c r="AK20" s="1">
-        <v>13</v>
+        <v>0.15051600000000001</v>
       </c>
       <c r="AL20" s="1">
-        <v>43</v>
-      </c>
-      <c r="AM20" s="1">
-        <v>0.36592400000000003</v>
-      </c>
-      <c r="AN20" s="1">
-        <v>0.337231</v>
-      </c>
-      <c r="AO20" s="1">
-        <v>0.122171</v>
-      </c>
-      <c r="AP20" s="1">
-        <v>0.15051600000000001</v>
-      </c>
-      <c r="AQ20" s="1">
         <v>0.79739599999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1">
         <v>100</v>
@@ -3203,117 +2888,102 @@
         <v>0.776362</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>11.662079</v>
       </c>
       <c r="J21" s="1">
-        <v>0</v>
+        <v>11.393286</v>
       </c>
       <c r="K21" s="1">
-        <v>0</v>
+        <v>3.099628</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>5.9026110000000003</v>
       </c>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>19.782284000000001</v>
       </c>
       <c r="N21" s="1">
-        <v>11.662079</v>
+        <v>5.0050999999999997</v>
       </c>
       <c r="O21" s="1">
-        <v>11.393286</v>
+        <v>4.6980000000000004</v>
       </c>
       <c r="P21" s="1">
-        <v>3.099628</v>
+        <v>2.5747</v>
       </c>
       <c r="Q21" s="1">
-        <v>5.9026110000000003</v>
+        <v>0.2059</v>
       </c>
       <c r="R21" s="1">
-        <v>19.782284000000001</v>
+        <v>10.9183</v>
       </c>
       <c r="S21" s="1">
-        <v>5.0050999999999997</v>
+        <v>6.7637</v>
       </c>
       <c r="T21" s="1">
-        <v>4.6980000000000004</v>
+        <v>6.6220999999999997</v>
       </c>
       <c r="U21" s="1">
-        <v>2.5747</v>
+        <v>2.7119</v>
       </c>
       <c r="V21" s="1">
-        <v>0.2059</v>
+        <v>0.38990000000000002</v>
       </c>
       <c r="W21" s="1">
-        <v>10.9183</v>
+        <v>12.861499999999999</v>
       </c>
       <c r="X21" s="1">
-        <v>6.7637</v>
+        <v>11.2424</v>
       </c>
       <c r="Y21" s="1">
-        <v>6.6220999999999997</v>
+        <v>11.068</v>
       </c>
       <c r="Z21" s="1">
-        <v>2.7119</v>
+        <v>1.6967000000000001</v>
       </c>
       <c r="AA21" s="1">
-        <v>0.38990000000000002</v>
+        <v>5.8789999999999996</v>
       </c>
       <c r="AB21" s="1">
-        <v>12.861499999999999</v>
+        <v>15.2776</v>
       </c>
       <c r="AC21" s="1">
-        <v>11.2424</v>
+        <v>30.32</v>
       </c>
       <c r="AD21" s="1">
-        <v>11.068</v>
+        <v>30</v>
       </c>
       <c r="AE21" s="1">
-        <v>1.6967000000000001</v>
+        <v>5.8756000000000004</v>
       </c>
       <c r="AF21" s="1">
-        <v>5.8789999999999996</v>
+        <v>15</v>
       </c>
       <c r="AG21" s="1">
-        <v>15.2776</v>
+        <v>43</v>
       </c>
       <c r="AH21" s="1">
-        <v>30.32</v>
+        <v>0.27969500000000003</v>
       </c>
       <c r="AI21" s="1">
-        <v>30</v>
+        <v>0.26080100000000001</v>
       </c>
       <c r="AJ21" s="1">
-        <v>5.8756000000000004</v>
+        <v>8.1642000000000006E-2</v>
       </c>
       <c r="AK21" s="1">
-        <v>15</v>
+        <v>0.104861</v>
       </c>
       <c r="AL21" s="1">
-        <v>43</v>
-      </c>
-      <c r="AM21" s="1">
-        <v>0.27969500000000003</v>
-      </c>
-      <c r="AN21" s="1">
-        <v>0.26080100000000001</v>
-      </c>
-      <c r="AO21" s="1">
-        <v>8.1642000000000006E-2</v>
-      </c>
-      <c r="AP21" s="1">
-        <v>0.104861</v>
-      </c>
-      <c r="AQ21" s="1">
         <v>0.53250600000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1">
         <v>100</v>
@@ -3334,117 +3004,102 @@
         <v>0.78838299999999994</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>10.043189</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>9.6672220000000006</v>
       </c>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>2.4522349999999999</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>6.2322790000000001</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
+        <v>16.985401</v>
       </c>
       <c r="N22" s="1">
-        <v>10.043189</v>
+        <v>3.9525000000000001</v>
       </c>
       <c r="O22" s="1">
-        <v>9.6672220000000006</v>
+        <v>3.6436000000000002</v>
       </c>
       <c r="P22" s="1">
-        <v>2.4522349999999999</v>
+        <v>2.1652</v>
       </c>
       <c r="Q22" s="1">
-        <v>6.2322790000000001</v>
+        <v>0.1016</v>
       </c>
       <c r="R22" s="1">
-        <v>16.985401</v>
+        <v>9.5906000000000002</v>
       </c>
       <c r="S22" s="1">
-        <v>3.9525000000000001</v>
+        <v>5.4507000000000003</v>
       </c>
       <c r="T22" s="1">
-        <v>3.6436000000000002</v>
+        <v>5.4741999999999997</v>
       </c>
       <c r="U22" s="1">
-        <v>2.1652</v>
+        <v>2.024</v>
       </c>
       <c r="V22" s="1">
-        <v>0.1016</v>
+        <v>0.30609999999999998</v>
       </c>
       <c r="W22" s="1">
-        <v>9.5906000000000002</v>
+        <v>10.778600000000001</v>
       </c>
       <c r="X22" s="1">
-        <v>5.4507000000000003</v>
+        <v>11.0357</v>
       </c>
       <c r="Y22" s="1">
-        <v>5.4741999999999997</v>
+        <v>11.133900000000001</v>
       </c>
       <c r="Z22" s="1">
-        <v>2.024</v>
+        <v>1.6529</v>
       </c>
       <c r="AA22" s="1">
-        <v>0.30609999999999998</v>
+        <v>7.9726999999999997</v>
       </c>
       <c r="AB22" s="1">
-        <v>10.778600000000001</v>
+        <v>17.771799999999999</v>
       </c>
       <c r="AC22" s="1">
-        <v>11.0357</v>
+        <v>28.73</v>
       </c>
       <c r="AD22" s="1">
-        <v>11.133900000000001</v>
+        <v>29</v>
       </c>
       <c r="AE22" s="1">
-        <v>1.6529</v>
+        <v>5.532</v>
       </c>
       <c r="AF22" s="1">
-        <v>7.9726999999999997</v>
+        <v>17</v>
       </c>
       <c r="AG22" s="1">
-        <v>17.771799999999999</v>
+        <v>42</v>
       </c>
       <c r="AH22" s="1">
-        <v>28.73</v>
+        <v>0.38073499999999999</v>
       </c>
       <c r="AI22" s="1">
-        <v>29</v>
+        <v>0.36139900000000003</v>
       </c>
       <c r="AJ22" s="1">
-        <v>5.532</v>
+        <v>0.114415</v>
       </c>
       <c r="AK22" s="1">
-        <v>17</v>
+        <v>0.16550699999999999</v>
       </c>
       <c r="AL22" s="1">
-        <v>42</v>
-      </c>
-      <c r="AM22" s="1">
-        <v>0.38073499999999999</v>
-      </c>
-      <c r="AN22" s="1">
-        <v>0.36139900000000003</v>
-      </c>
-      <c r="AO22" s="1">
-        <v>0.114415</v>
-      </c>
-      <c r="AP22" s="1">
-        <v>0.16550699999999999</v>
-      </c>
-      <c r="AQ22" s="1">
         <v>0.719526</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>100</v>
@@ -3465,117 +3120,102 @@
         <v>0.78301699999999996</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>11.117001</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>10.634575999999999</v>
       </c>
       <c r="K23" s="1">
-        <v>0</v>
+        <v>3.0820910000000001</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>5.6461610000000002</v>
       </c>
       <c r="M23" s="1">
-        <v>0</v>
+        <v>20.635801000000001</v>
       </c>
       <c r="N23" s="1">
-        <v>11.117001</v>
+        <v>4.5685000000000002</v>
       </c>
       <c r="O23" s="1">
-        <v>10.634575999999999</v>
+        <v>4.3581000000000003</v>
       </c>
       <c r="P23" s="1">
-        <v>3.0820910000000001</v>
+        <v>2.6604999999999999</v>
       </c>
       <c r="Q23" s="1">
-        <v>5.6461610000000002</v>
+        <v>3.6200000000000003E-2</v>
       </c>
       <c r="R23" s="1">
-        <v>20.635801000000001</v>
+        <v>12.8057</v>
       </c>
       <c r="S23" s="1">
-        <v>4.5685000000000002</v>
+        <v>6.3227000000000002</v>
       </c>
       <c r="T23" s="1">
-        <v>4.3581000000000003</v>
+        <v>6.3113999999999999</v>
       </c>
       <c r="U23" s="1">
-        <v>2.6604999999999999</v>
+        <v>2.6657999999999999</v>
       </c>
       <c r="V23" s="1">
-        <v>3.6200000000000003E-2</v>
+        <v>0.1036</v>
       </c>
       <c r="W23" s="1">
-        <v>12.8057</v>
+        <v>13.568</v>
       </c>
       <c r="X23" s="1">
-        <v>6.3227000000000002</v>
+        <v>11.3916</v>
       </c>
       <c r="Y23" s="1">
-        <v>6.3113999999999999</v>
+        <v>11.0327</v>
       </c>
       <c r="Z23" s="1">
-        <v>2.6657999999999999</v>
+        <v>1.8972</v>
       </c>
       <c r="AA23" s="1">
-        <v>0.1036</v>
+        <v>7.9253999999999998</v>
       </c>
       <c r="AB23" s="1">
-        <v>13.568</v>
+        <v>16.085999999999999</v>
       </c>
       <c r="AC23" s="1">
-        <v>11.3916</v>
+        <v>31.2</v>
       </c>
       <c r="AD23" s="1">
-        <v>11.0327</v>
+        <v>30</v>
       </c>
       <c r="AE23" s="1">
-        <v>1.8972</v>
+        <v>5.7611999999999997</v>
       </c>
       <c r="AF23" s="1">
-        <v>7.9253999999999998</v>
+        <v>19</v>
       </c>
       <c r="AG23" s="1">
-        <v>16.085999999999999</v>
+        <v>48</v>
       </c>
       <c r="AH23" s="1">
-        <v>31.2</v>
+        <v>0.29247800000000002</v>
       </c>
       <c r="AI23" s="1">
-        <v>30</v>
+        <v>0.274399</v>
       </c>
       <c r="AJ23" s="1">
-        <v>5.7611999999999997</v>
+        <v>7.6324000000000003E-2</v>
       </c>
       <c r="AK23" s="1">
-        <v>19</v>
+        <v>0.16394700000000001</v>
       </c>
       <c r="AL23" s="1">
-        <v>48</v>
-      </c>
-      <c r="AM23" s="1">
-        <v>0.29247800000000002</v>
-      </c>
-      <c r="AN23" s="1">
-        <v>0.274399</v>
-      </c>
-      <c r="AO23" s="1">
-        <v>7.6324000000000003E-2</v>
-      </c>
-      <c r="AP23" s="1">
-        <v>0.16394700000000001</v>
-      </c>
-      <c r="AQ23" s="1">
         <v>0.54440900000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1">
         <v>100</v>
@@ -3596,117 +3236,102 @@
         <v>0.76796500000000001</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>10.548397</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>10.391002</v>
       </c>
       <c r="K24" s="1">
-        <v>0</v>
+        <v>2.411467</v>
       </c>
       <c r="L24" s="1">
-        <v>0</v>
+        <v>5.93222</v>
       </c>
       <c r="M24" s="1">
-        <v>0</v>
+        <v>18.452850000000002</v>
       </c>
       <c r="N24" s="1">
-        <v>10.548397</v>
+        <v>4.2998000000000003</v>
       </c>
       <c r="O24" s="1">
-        <v>10.391002</v>
+        <v>4.0686</v>
       </c>
       <c r="P24" s="1">
-        <v>2.411467</v>
+        <v>2.2736999999999998</v>
       </c>
       <c r="Q24" s="1">
-        <v>5.93222</v>
+        <v>8.9700000000000002E-2</v>
       </c>
       <c r="R24" s="1">
-        <v>18.452850000000002</v>
+        <v>13.5685</v>
       </c>
       <c r="S24" s="1">
-        <v>4.2998000000000003</v>
+        <v>5.6078000000000001</v>
       </c>
       <c r="T24" s="1">
-        <v>4.0686</v>
+        <v>5.4927999999999999</v>
       </c>
       <c r="U24" s="1">
-        <v>2.2736999999999998</v>
+        <v>2.1964000000000001</v>
       </c>
       <c r="V24" s="1">
-        <v>8.9700000000000002E-2</v>
+        <v>0.83989999999999998</v>
       </c>
       <c r="W24" s="1">
-        <v>13.5685</v>
+        <v>12.924099999999999</v>
       </c>
       <c r="X24" s="1">
-        <v>5.6078000000000001</v>
+        <v>11.317500000000001</v>
       </c>
       <c r="Y24" s="1">
-        <v>5.4927999999999999</v>
+        <v>11.2836</v>
       </c>
       <c r="Z24" s="1">
-        <v>2.1964000000000001</v>
+        <v>1.5162</v>
       </c>
       <c r="AA24" s="1">
-        <v>0.83989999999999998</v>
+        <v>8.3096999999999994</v>
       </c>
       <c r="AB24" s="1">
-        <v>12.924099999999999</v>
+        <v>15.4062</v>
       </c>
       <c r="AC24" s="1">
-        <v>11.317500000000001</v>
+        <v>28.79</v>
       </c>
       <c r="AD24" s="1">
-        <v>11.2836</v>
+        <v>29</v>
       </c>
       <c r="AE24" s="1">
-        <v>1.5162</v>
+        <v>5.2518000000000002</v>
       </c>
       <c r="AF24" s="1">
-        <v>8.3096999999999994</v>
+        <v>16</v>
       </c>
       <c r="AG24" s="1">
-        <v>15.4062</v>
+        <v>45</v>
       </c>
       <c r="AH24" s="1">
-        <v>28.79</v>
+        <v>0.39918399999999998</v>
       </c>
       <c r="AI24" s="1">
-        <v>29</v>
+        <v>0.37070799999999998</v>
       </c>
       <c r="AJ24" s="1">
-        <v>5.2518000000000002</v>
+        <v>0.11515300000000001</v>
       </c>
       <c r="AK24" s="1">
-        <v>16</v>
+        <v>0.18205299999999999</v>
       </c>
       <c r="AL24" s="1">
-        <v>45</v>
-      </c>
-      <c r="AM24" s="1">
-        <v>0.39918399999999998</v>
-      </c>
-      <c r="AN24" s="1">
-        <v>0.37070799999999998</v>
-      </c>
-      <c r="AO24" s="1">
-        <v>0.11515300000000001</v>
-      </c>
-      <c r="AP24" s="1">
-        <v>0.18205299999999999</v>
-      </c>
-      <c r="AQ24" s="1">
         <v>0.70336699999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1">
         <v>100</v>
@@ -3727,117 +3352,102 @@
         <v>0.74669200000000002</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>11.473490999999999</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <v>11.286911</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>2.6999659999999999</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>5.8978339999999996</v>
       </c>
       <c r="M25" s="1">
-        <v>0</v>
+        <v>19.321570000000001</v>
       </c>
       <c r="N25" s="1">
-        <v>11.473490999999999</v>
+        <v>4.5583</v>
       </c>
       <c r="O25" s="1">
-        <v>11.286911</v>
+        <v>4.2394999999999996</v>
       </c>
       <c r="P25" s="1">
-        <v>2.6999659999999999</v>
+        <v>2.5145</v>
       </c>
       <c r="Q25" s="1">
-        <v>5.8978339999999996</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="R25" s="1">
-        <v>19.321570000000001</v>
+        <v>13.3775</v>
       </c>
       <c r="S25" s="1">
-        <v>4.5583</v>
+        <v>7.1036999999999999</v>
       </c>
       <c r="T25" s="1">
-        <v>4.2394999999999996</v>
+        <v>7.2095000000000002</v>
       </c>
       <c r="U25" s="1">
-        <v>2.5145</v>
+        <v>2.4388999999999998</v>
       </c>
       <c r="V25" s="1">
-        <v>0.14749999999999999</v>
+        <v>0.87370000000000003</v>
       </c>
       <c r="W25" s="1">
-        <v>13.3775</v>
+        <v>13.1267</v>
       </c>
       <c r="X25" s="1">
-        <v>7.1036999999999999</v>
+        <v>11.5641</v>
       </c>
       <c r="Y25" s="1">
-        <v>7.2095000000000002</v>
+        <v>11.5678</v>
       </c>
       <c r="Z25" s="1">
-        <v>2.4388999999999998</v>
+        <v>1.4211</v>
       </c>
       <c r="AA25" s="1">
-        <v>0.87370000000000003</v>
+        <v>8.0695999999999994</v>
       </c>
       <c r="AB25" s="1">
-        <v>13.1267</v>
+        <v>15.523099999999999</v>
       </c>
       <c r="AC25" s="1">
-        <v>11.5641</v>
+        <v>32.119999999999997</v>
       </c>
       <c r="AD25" s="1">
-        <v>11.5678</v>
+        <v>31.5</v>
       </c>
       <c r="AE25" s="1">
-        <v>1.4211</v>
+        <v>6.2994000000000003</v>
       </c>
       <c r="AF25" s="1">
-        <v>8.0695999999999994</v>
+        <v>21</v>
       </c>
       <c r="AG25" s="1">
-        <v>15.523099999999999</v>
+        <v>54</v>
       </c>
       <c r="AH25" s="1">
-        <v>32.119999999999997</v>
+        <v>0.31070399999999998</v>
       </c>
       <c r="AI25" s="1">
-        <v>31.5</v>
+        <v>0.29705300000000001</v>
       </c>
       <c r="AJ25" s="1">
-        <v>6.2994000000000003</v>
+        <v>8.1060999999999994E-2</v>
       </c>
       <c r="AK25" s="1">
-        <v>21</v>
+        <v>0.141407</v>
       </c>
       <c r="AL25" s="1">
-        <v>54</v>
-      </c>
-      <c r="AM25" s="1">
-        <v>0.31070399999999998</v>
-      </c>
-      <c r="AN25" s="1">
-        <v>0.29705300000000001</v>
-      </c>
-      <c r="AO25" s="1">
-        <v>8.1060999999999994E-2</v>
-      </c>
-      <c r="AP25" s="1">
-        <v>0.141407</v>
-      </c>
-      <c r="AQ25" s="1">
         <v>0.511347</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1">
         <v>100</v>
@@ -3858,117 +3468,102 @@
         <v>0.76302499999999995</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>10.306900000000001</v>
       </c>
       <c r="J26" s="1">
-        <v>0</v>
+        <v>10.170090999999999</v>
       </c>
       <c r="K26" s="1">
-        <v>0</v>
+        <v>2.334454</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>5.7710520000000001</v>
       </c>
       <c r="M26" s="1">
-        <v>0</v>
+        <v>16.875043999999999</v>
       </c>
       <c r="N26" s="1">
-        <v>10.306900000000001</v>
+        <v>4.2416</v>
       </c>
       <c r="O26" s="1">
-        <v>10.170090999999999</v>
+        <v>4.0536000000000003</v>
       </c>
       <c r="P26" s="1">
-        <v>2.334454</v>
+        <v>2.0455999999999999</v>
       </c>
       <c r="Q26" s="1">
-        <v>5.7710520000000001</v>
+        <v>0.1173</v>
       </c>
       <c r="R26" s="1">
-        <v>16.875043999999999</v>
+        <v>11.052300000000001</v>
       </c>
       <c r="S26" s="1">
-        <v>4.2416</v>
+        <v>5.4482999999999997</v>
       </c>
       <c r="T26" s="1">
-        <v>4.0536000000000003</v>
+        <v>5.3661000000000003</v>
       </c>
       <c r="U26" s="1">
-        <v>2.0455999999999999</v>
+        <v>1.9288000000000001</v>
       </c>
       <c r="V26" s="1">
-        <v>0.1173</v>
+        <v>0.32029999999999997</v>
       </c>
       <c r="W26" s="1">
-        <v>11.052300000000001</v>
+        <v>10.3407</v>
       </c>
       <c r="X26" s="1">
-        <v>5.4482999999999997</v>
+        <v>10.983499999999999</v>
       </c>
       <c r="Y26" s="1">
-        <v>5.3661000000000003</v>
+        <v>10.8802</v>
       </c>
       <c r="Z26" s="1">
-        <v>1.9288000000000001</v>
+        <v>1.3528</v>
       </c>
       <c r="AA26" s="1">
-        <v>0.32029999999999997</v>
+        <v>7.9623999999999997</v>
       </c>
       <c r="AB26" s="1">
-        <v>10.3407</v>
+        <v>14.648300000000001</v>
       </c>
       <c r="AC26" s="1">
-        <v>10.983499999999999</v>
+        <v>28.69</v>
       </c>
       <c r="AD26" s="1">
-        <v>10.8802</v>
+        <v>29</v>
       </c>
       <c r="AE26" s="1">
-        <v>1.3528</v>
+        <v>5.2679999999999998</v>
       </c>
       <c r="AF26" s="1">
-        <v>7.9623999999999997</v>
+        <v>16</v>
       </c>
       <c r="AG26" s="1">
-        <v>14.648300000000001</v>
+        <v>45</v>
       </c>
       <c r="AH26" s="1">
-        <v>28.69</v>
+        <v>0.42743300000000001</v>
       </c>
       <c r="AI26" s="1">
-        <v>29</v>
+        <v>0.427838</v>
       </c>
       <c r="AJ26" s="1">
-        <v>5.2679999999999998</v>
+        <v>0.113652</v>
       </c>
       <c r="AK26" s="1">
-        <v>16</v>
+        <v>0.22384799999999999</v>
       </c>
       <c r="AL26" s="1">
-        <v>45</v>
-      </c>
-      <c r="AM26" s="1">
-        <v>0.42743300000000001</v>
-      </c>
-      <c r="AN26" s="1">
-        <v>0.427838</v>
-      </c>
-      <c r="AO26" s="1">
-        <v>0.113652</v>
-      </c>
-      <c r="AP26" s="1">
-        <v>0.22384799999999999</v>
-      </c>
-      <c r="AQ26" s="1">
         <v>0.77346199999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1">
         <v>100</v>
@@ -3989,117 +3584,102 @@
         <v>0.74463599999999996</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>11.042051000000001</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
+        <v>10.510127000000001</v>
       </c>
       <c r="K27" s="1">
-        <v>0</v>
+        <v>2.5071479999999999</v>
       </c>
       <c r="L27" s="1">
-        <v>0</v>
+        <v>6.4297180000000003</v>
       </c>
       <c r="M27" s="1">
-        <v>0</v>
+        <v>18.504812000000001</v>
       </c>
       <c r="N27" s="1">
-        <v>11.042051000000001</v>
+        <v>4.3209</v>
       </c>
       <c r="O27" s="1">
-        <v>10.510127000000001</v>
+        <v>4.1521999999999997</v>
       </c>
       <c r="P27" s="1">
-        <v>2.5071479999999999</v>
+        <v>2.4777999999999998</v>
       </c>
       <c r="Q27" s="1">
-        <v>6.4297180000000003</v>
+        <v>0.1389</v>
       </c>
       <c r="R27" s="1">
-        <v>18.504812000000001</v>
+        <v>13.457800000000001</v>
       </c>
       <c r="S27" s="1">
-        <v>4.3209</v>
+        <v>6.5304000000000002</v>
       </c>
       <c r="T27" s="1">
-        <v>4.1521999999999997</v>
+        <v>6.6454000000000004</v>
       </c>
       <c r="U27" s="1">
-        <v>2.4777999999999998</v>
+        <v>2.5266999999999999</v>
       </c>
       <c r="V27" s="1">
-        <v>0.1389</v>
+        <v>0.82179999999999997</v>
       </c>
       <c r="W27" s="1">
-        <v>13.457800000000001</v>
+        <v>11.4125</v>
       </c>
       <c r="X27" s="1">
-        <v>6.5304000000000002</v>
+        <v>11.6302</v>
       </c>
       <c r="Y27" s="1">
-        <v>6.6454000000000004</v>
+        <v>11.8864</v>
       </c>
       <c r="Z27" s="1">
-        <v>2.5266999999999999</v>
+        <v>1.6228</v>
       </c>
       <c r="AA27" s="1">
-        <v>0.82179999999999997</v>
+        <v>7.5884999999999998</v>
       </c>
       <c r="AB27" s="1">
-        <v>11.4125</v>
+        <v>15.5649</v>
       </c>
       <c r="AC27" s="1">
-        <v>11.6302</v>
+        <v>32.229999999999997</v>
       </c>
       <c r="AD27" s="1">
-        <v>11.8864</v>
+        <v>32</v>
       </c>
       <c r="AE27" s="1">
-        <v>1.6228</v>
+        <v>6.0716999999999999</v>
       </c>
       <c r="AF27" s="1">
-        <v>7.5884999999999998</v>
+        <v>19</v>
       </c>
       <c r="AG27" s="1">
-        <v>15.5649</v>
+        <v>55</v>
       </c>
       <c r="AH27" s="1">
-        <v>32.229999999999997</v>
+        <v>0.33616099999999999</v>
       </c>
       <c r="AI27" s="1">
-        <v>32</v>
+        <v>0.32054700000000003</v>
       </c>
       <c r="AJ27" s="1">
-        <v>6.0716999999999999</v>
+        <v>8.9418999999999998E-2</v>
       </c>
       <c r="AK27" s="1">
-        <v>19</v>
+        <v>0.17163100000000001</v>
       </c>
       <c r="AL27" s="1">
-        <v>55</v>
-      </c>
-      <c r="AM27" s="1">
-        <v>0.33616099999999999</v>
-      </c>
-      <c r="AN27" s="1">
-        <v>0.32054700000000003</v>
-      </c>
-      <c r="AO27" s="1">
-        <v>8.9418999999999998E-2</v>
-      </c>
-      <c r="AP27" s="1">
-        <v>0.17163100000000001</v>
-      </c>
-      <c r="AQ27" s="1">
         <v>0.61008300000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1">
         <v>100</v>
@@ -4120,117 +3700,102 @@
         <v>0.77666900000000005</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>9.8913189999999993</v>
       </c>
       <c r="J28" s="1">
-        <v>0</v>
+        <v>9.754232</v>
       </c>
       <c r="K28" s="1">
-        <v>0</v>
+        <v>2.400509</v>
       </c>
       <c r="L28" s="1">
-        <v>0</v>
+        <v>4.7531540000000003</v>
       </c>
       <c r="M28" s="1">
-        <v>0</v>
+        <v>16.384979000000001</v>
       </c>
       <c r="N28" s="1">
-        <v>9.8913189999999993</v>
+        <v>3.7545000000000002</v>
       </c>
       <c r="O28" s="1">
-        <v>9.754232</v>
+        <v>3.8102</v>
       </c>
       <c r="P28" s="1">
-        <v>2.400509</v>
+        <v>2.2111000000000001</v>
       </c>
       <c r="Q28" s="1">
-        <v>4.7531540000000003</v>
+        <v>5.91E-2</v>
       </c>
       <c r="R28" s="1">
-        <v>16.384979000000001</v>
+        <v>11.541</v>
       </c>
       <c r="S28" s="1">
-        <v>3.7545000000000002</v>
+        <v>5.4676999999999998</v>
       </c>
       <c r="T28" s="1">
-        <v>3.8102</v>
+        <v>5.6920999999999999</v>
       </c>
       <c r="U28" s="1">
-        <v>2.2111000000000001</v>
+        <v>2.4561999999999999</v>
       </c>
       <c r="V28" s="1">
-        <v>5.91E-2</v>
+        <v>2.58E-2</v>
       </c>
       <c r="W28" s="1">
-        <v>11.541</v>
+        <v>12.0099</v>
       </c>
       <c r="X28" s="1">
-        <v>5.4676999999999998</v>
+        <v>11.133699999999999</v>
       </c>
       <c r="Y28" s="1">
-        <v>5.6920999999999999</v>
+        <v>11.151</v>
       </c>
       <c r="Z28" s="1">
-        <v>2.4561999999999999</v>
+        <v>1.4039999999999999</v>
       </c>
       <c r="AA28" s="1">
-        <v>2.58E-2</v>
+        <v>7.4024000000000001</v>
       </c>
       <c r="AB28" s="1">
-        <v>12.0099</v>
+        <v>15.341100000000001</v>
       </c>
       <c r="AC28" s="1">
-        <v>11.133699999999999</v>
+        <v>29.49</v>
       </c>
       <c r="AD28" s="1">
-        <v>11.151</v>
+        <v>29</v>
       </c>
       <c r="AE28" s="1">
-        <v>1.4039999999999999</v>
+        <v>5.3342999999999998</v>
       </c>
       <c r="AF28" s="1">
-        <v>7.4024000000000001</v>
+        <v>17</v>
       </c>
       <c r="AG28" s="1">
-        <v>15.341100000000001</v>
+        <v>42</v>
       </c>
       <c r="AH28" s="1">
-        <v>29.49</v>
+        <v>0.44870599999999999</v>
       </c>
       <c r="AI28" s="1">
-        <v>29</v>
+        <v>0.43421399999999999</v>
       </c>
       <c r="AJ28" s="1">
-        <v>5.3342999999999998</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="AK28" s="1">
-        <v>17</v>
+        <v>0.256471</v>
       </c>
       <c r="AL28" s="1">
-        <v>42</v>
-      </c>
-      <c r="AM28" s="1">
-        <v>0.44870599999999999</v>
-      </c>
-      <c r="AN28" s="1">
-        <v>0.43421399999999999</v>
-      </c>
-      <c r="AO28" s="1">
-        <v>0.13125000000000001</v>
-      </c>
-      <c r="AP28" s="1">
-        <v>0.256471</v>
-      </c>
-      <c r="AQ28" s="1">
         <v>1.020518</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1">
         <v>100</v>
@@ -4251,117 +3816,102 @@
         <v>0.73231800000000002</v>
       </c>
       <c r="I29" s="1">
-        <v>0</v>
+        <v>11.066314999999999</v>
       </c>
       <c r="J29" s="1">
-        <v>0</v>
+        <v>10.771641000000001</v>
       </c>
       <c r="K29" s="1">
-        <v>0</v>
+        <v>2.5192239999999999</v>
       </c>
       <c r="L29" s="1">
-        <v>0</v>
+        <v>5.5643500000000001</v>
       </c>
       <c r="M29" s="1">
-        <v>0</v>
+        <v>18.868476000000001</v>
       </c>
       <c r="N29" s="1">
-        <v>11.066314999999999</v>
+        <v>4.3061999999999996</v>
       </c>
       <c r="O29" s="1">
-        <v>10.771641000000001</v>
+        <v>4.1919000000000004</v>
       </c>
       <c r="P29" s="1">
-        <v>2.5192239999999999</v>
+        <v>2.2025000000000001</v>
       </c>
       <c r="Q29" s="1">
-        <v>5.5643500000000001</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="R29" s="1">
-        <v>18.868476000000001</v>
+        <v>10.751300000000001</v>
       </c>
       <c r="S29" s="1">
-        <v>4.3061999999999996</v>
+        <v>6.8055000000000003</v>
       </c>
       <c r="T29" s="1">
-        <v>4.1919000000000004</v>
+        <v>6.7876000000000003</v>
       </c>
       <c r="U29" s="1">
-        <v>2.2025000000000001</v>
+        <v>2.3565</v>
       </c>
       <c r="V29" s="1">
-        <v>4.6899999999999997E-2</v>
+        <v>0.73380000000000001</v>
       </c>
       <c r="W29" s="1">
-        <v>10.751300000000001</v>
+        <v>12.8194</v>
       </c>
       <c r="X29" s="1">
-        <v>6.8055000000000003</v>
+        <v>11.4444</v>
       </c>
       <c r="Y29" s="1">
-        <v>6.7876000000000003</v>
+        <v>11.4374</v>
       </c>
       <c r="Z29" s="1">
-        <v>2.3565</v>
+        <v>1.5920000000000001</v>
       </c>
       <c r="AA29" s="1">
-        <v>0.73380000000000001</v>
+        <v>7.8452999999999999</v>
       </c>
       <c r="AB29" s="1">
-        <v>12.8194</v>
+        <v>15.2476</v>
       </c>
       <c r="AC29" s="1">
-        <v>11.4444</v>
+        <v>32.74</v>
       </c>
       <c r="AD29" s="1">
-        <v>11.4374</v>
+        <v>32</v>
       </c>
       <c r="AE29" s="1">
-        <v>1.5920000000000001</v>
+        <v>5.0605000000000002</v>
       </c>
       <c r="AF29" s="1">
-        <v>7.8452999999999999</v>
+        <v>23</v>
       </c>
       <c r="AG29" s="1">
-        <v>15.2476</v>
+        <v>48</v>
       </c>
       <c r="AH29" s="1">
-        <v>32.74</v>
+        <v>0.338142</v>
       </c>
       <c r="AI29" s="1">
-        <v>32</v>
+        <v>0.32895400000000002</v>
       </c>
       <c r="AJ29" s="1">
-        <v>5.0605000000000002</v>
+        <v>8.0620999999999998E-2</v>
       </c>
       <c r="AK29" s="1">
-        <v>23</v>
+        <v>0.19818</v>
       </c>
       <c r="AL29" s="1">
-        <v>48</v>
-      </c>
-      <c r="AM29" s="1">
-        <v>0.338142</v>
-      </c>
-      <c r="AN29" s="1">
-        <v>0.32895400000000002</v>
-      </c>
-      <c r="AO29" s="1">
-        <v>8.0620999999999998E-2</v>
-      </c>
-      <c r="AP29" s="1">
-        <v>0.19818</v>
-      </c>
-      <c r="AQ29" s="1">
         <v>0.55429700000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1">
         <v>100</v>
@@ -4382,117 +3932,102 @@
         <v>0.77538200000000002</v>
       </c>
       <c r="I30" s="1">
-        <v>0</v>
+        <v>9.683287</v>
       </c>
       <c r="J30" s="1">
-        <v>0</v>
+        <v>9.4763129999999993</v>
       </c>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>2.2094339999999999</v>
       </c>
       <c r="L30" s="1">
-        <v>0</v>
+        <v>5.5818329999999996</v>
       </c>
       <c r="M30" s="1">
-        <v>0</v>
+        <v>16.880395</v>
       </c>
       <c r="N30" s="1">
-        <v>9.683287</v>
+        <v>3.6280999999999999</v>
       </c>
       <c r="O30" s="1">
-        <v>9.4763129999999993</v>
+        <v>3.4626999999999999</v>
       </c>
       <c r="P30" s="1">
-        <v>2.2094339999999999</v>
+        <v>1.8614999999999999</v>
       </c>
       <c r="Q30" s="1">
-        <v>5.5818329999999996</v>
+        <v>3.9899999999999998E-2</v>
       </c>
       <c r="R30" s="1">
-        <v>16.880395</v>
+        <v>8.7995999999999999</v>
       </c>
       <c r="S30" s="1">
-        <v>3.6280999999999999</v>
+        <v>5.1227</v>
       </c>
       <c r="T30" s="1">
-        <v>3.4626999999999999</v>
+        <v>5.22</v>
       </c>
       <c r="U30" s="1">
-        <v>1.8614999999999999</v>
+        <v>2.0184000000000002</v>
       </c>
       <c r="V30" s="1">
-        <v>3.9899999999999998E-2</v>
+        <v>0.31330000000000002</v>
       </c>
       <c r="W30" s="1">
-        <v>8.7995999999999999</v>
+        <v>9.5851000000000006</v>
       </c>
       <c r="X30" s="1">
-        <v>5.1227</v>
+        <v>11.270099999999999</v>
       </c>
       <c r="Y30" s="1">
-        <v>5.22</v>
+        <v>11.276899999999999</v>
       </c>
       <c r="Z30" s="1">
-        <v>2.0184000000000002</v>
+        <v>1.6415999999999999</v>
       </c>
       <c r="AA30" s="1">
-        <v>0.31330000000000002</v>
+        <v>7.0979000000000001</v>
       </c>
       <c r="AB30" s="1">
-        <v>9.5851000000000006</v>
+        <v>15.950699999999999</v>
       </c>
       <c r="AC30" s="1">
-        <v>11.270099999999999</v>
+        <v>28.8</v>
       </c>
       <c r="AD30" s="1">
-        <v>11.276899999999999</v>
+        <v>29</v>
       </c>
       <c r="AE30" s="1">
-        <v>1.6415999999999999</v>
+        <v>4.5946999999999996</v>
       </c>
       <c r="AF30" s="1">
-        <v>7.0979000000000001</v>
+        <v>20</v>
       </c>
       <c r="AG30" s="1">
-        <v>15.950699999999999</v>
+        <v>45</v>
       </c>
       <c r="AH30" s="1">
-        <v>28.8</v>
+        <v>0.44850400000000001</v>
       </c>
       <c r="AI30" s="1">
-        <v>29</v>
+        <v>0.41738500000000001</v>
       </c>
       <c r="AJ30" s="1">
-        <v>4.5946999999999996</v>
+        <v>0.106336</v>
       </c>
       <c r="AK30" s="1">
-        <v>20</v>
+        <v>0.274976</v>
       </c>
       <c r="AL30" s="1">
-        <v>45</v>
-      </c>
-      <c r="AM30" s="1">
-        <v>0.44850400000000001</v>
-      </c>
-      <c r="AN30" s="1">
-        <v>0.41738500000000001</v>
-      </c>
-      <c r="AO30" s="1">
-        <v>0.106336</v>
-      </c>
-      <c r="AP30" s="1">
-        <v>0.274976</v>
-      </c>
-      <c r="AQ30" s="1">
         <v>0.79581000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1">
         <v>100</v>
@@ -4513,117 +4048,102 @@
         <v>0.73857200000000001</v>
       </c>
       <c r="I31" s="1">
-        <v>0</v>
+        <v>11.254034000000001</v>
       </c>
       <c r="J31" s="1">
-        <v>0</v>
+        <v>11.231602000000001</v>
       </c>
       <c r="K31" s="1">
-        <v>0</v>
+        <v>2.438367</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>6.5482069999999997</v>
       </c>
       <c r="M31" s="1">
-        <v>0</v>
+        <v>18.023415</v>
       </c>
       <c r="N31" s="1">
-        <v>11.254034000000001</v>
+        <v>4.2755999999999998</v>
       </c>
       <c r="O31" s="1">
-        <v>11.231602000000001</v>
+        <v>3.9977999999999998</v>
       </c>
       <c r="P31" s="1">
-        <v>2.438367</v>
+        <v>2.2433000000000001</v>
       </c>
       <c r="Q31" s="1">
-        <v>6.5482069999999997</v>
+        <v>0.33279999999999998</v>
       </c>
       <c r="R31" s="1">
-        <v>18.023415</v>
+        <v>10.902100000000001</v>
       </c>
       <c r="S31" s="1">
-        <v>4.2755999999999998</v>
+        <v>6.9996</v>
       </c>
       <c r="T31" s="1">
-        <v>3.9977999999999998</v>
+        <v>6.9097</v>
       </c>
       <c r="U31" s="1">
-        <v>2.2433000000000001</v>
+        <v>2.3298000000000001</v>
       </c>
       <c r="V31" s="1">
-        <v>0.33279999999999998</v>
+        <v>0.35959999999999998</v>
       </c>
       <c r="W31" s="1">
-        <v>10.902100000000001</v>
+        <v>13.385</v>
       </c>
       <c r="X31" s="1">
-        <v>6.9996</v>
+        <v>11.832800000000001</v>
       </c>
       <c r="Y31" s="1">
-        <v>6.9097</v>
+        <v>11.5579</v>
       </c>
       <c r="Z31" s="1">
-        <v>2.3298000000000001</v>
+        <v>1.7111000000000001</v>
       </c>
       <c r="AA31" s="1">
-        <v>0.35959999999999998</v>
+        <v>7.9961000000000002</v>
       </c>
       <c r="AB31" s="1">
-        <v>13.385</v>
+        <v>17.533899999999999</v>
       </c>
       <c r="AC31" s="1">
-        <v>11.832800000000001</v>
+        <v>33.47</v>
       </c>
       <c r="AD31" s="1">
-        <v>11.5579</v>
+        <v>33</v>
       </c>
       <c r="AE31" s="1">
-        <v>1.7111000000000001</v>
+        <v>5.5513000000000003</v>
       </c>
       <c r="AF31" s="1">
-        <v>7.9961000000000002</v>
+        <v>23</v>
       </c>
       <c r="AG31" s="1">
-        <v>17.533899999999999</v>
+        <v>55</v>
       </c>
       <c r="AH31" s="1">
-        <v>33.47</v>
+        <v>0.35105999999999998</v>
       </c>
       <c r="AI31" s="1">
-        <v>33</v>
+        <v>0.33153199999999999</v>
       </c>
       <c r="AJ31" s="1">
-        <v>5.5513000000000003</v>
+        <v>7.7719999999999997E-2</v>
       </c>
       <c r="AK31" s="1">
-        <v>23</v>
+        <v>0.211149</v>
       </c>
       <c r="AL31" s="1">
+        <v>0.53735100000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AM31" s="1">
-        <v>0.35105999999999998</v>
-      </c>
-      <c r="AN31" s="1">
-        <v>0.33153199999999999</v>
-      </c>
-      <c r="AO31" s="1">
-        <v>7.7719999999999997E-2</v>
-      </c>
-      <c r="AP31" s="1">
-        <v>0.211149</v>
-      </c>
-      <c r="AQ31" s="1">
-        <v>0.53735100000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1">
         <v>100</v>
@@ -4644,117 +4164,102 @@
         <v>0.76013799999999998</v>
       </c>
       <c r="I32" s="1">
-        <v>0</v>
+        <v>10.412374</v>
       </c>
       <c r="J32" s="1">
-        <v>0</v>
+        <v>10.578234999999999</v>
       </c>
       <c r="K32" s="1">
-        <v>0</v>
+        <v>2.2727439999999999</v>
       </c>
       <c r="L32" s="1">
-        <v>0</v>
+        <v>5.8739179999999998</v>
       </c>
       <c r="M32" s="1">
-        <v>0</v>
+        <v>16.172370000000001</v>
       </c>
       <c r="N32" s="1">
-        <v>10.412374</v>
+        <v>4.1060999999999996</v>
       </c>
       <c r="O32" s="1">
-        <v>10.578234999999999</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="P32" s="1">
-        <v>2.2727439999999999</v>
+        <v>2.0737999999999999</v>
       </c>
       <c r="Q32" s="1">
-        <v>5.8739179999999998</v>
+        <v>0.2243</v>
       </c>
       <c r="R32" s="1">
-        <v>16.172370000000001</v>
+        <v>9.4437999999999995</v>
       </c>
       <c r="S32" s="1">
-        <v>4.1060999999999996</v>
+        <v>5.5377000000000001</v>
       </c>
       <c r="T32" s="1">
-        <v>4.1500000000000004</v>
+        <v>5.5555000000000003</v>
       </c>
       <c r="U32" s="1">
-        <v>2.0737999999999999</v>
+        <v>2.1608999999999998</v>
       </c>
       <c r="V32" s="1">
-        <v>0.2243</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="W32" s="1">
-        <v>9.4437999999999995</v>
+        <v>11.2187</v>
       </c>
       <c r="X32" s="1">
-        <v>5.5377000000000001</v>
+        <v>11.539199999999999</v>
       </c>
       <c r="Y32" s="1">
-        <v>5.5555000000000003</v>
+        <v>11.4948</v>
       </c>
       <c r="Z32" s="1">
-        <v>2.1608999999999998</v>
+        <v>1.3725000000000001</v>
       </c>
       <c r="AA32" s="1">
-        <v>0.65600000000000003</v>
+        <v>8.0607000000000006</v>
       </c>
       <c r="AB32" s="1">
-        <v>11.2187</v>
+        <v>15.286199999999999</v>
       </c>
       <c r="AC32" s="1">
-        <v>11.539199999999999</v>
+        <v>29.42</v>
       </c>
       <c r="AD32" s="1">
-        <v>11.4948</v>
+        <v>29</v>
       </c>
       <c r="AE32" s="1">
-        <v>1.3725000000000001</v>
+        <v>4.6432000000000002</v>
       </c>
       <c r="AF32" s="1">
-        <v>8.0607000000000006</v>
+        <v>20</v>
       </c>
       <c r="AG32" s="1">
-        <v>15.286199999999999</v>
+        <v>43</v>
       </c>
       <c r="AH32" s="1">
-        <v>29.42</v>
+        <v>0.45260299999999998</v>
       </c>
       <c r="AI32" s="1">
-        <v>29</v>
+        <v>0.43103000000000002</v>
       </c>
       <c r="AJ32" s="1">
-        <v>4.6432000000000002</v>
+        <v>9.8665000000000003E-2</v>
       </c>
       <c r="AK32" s="1">
-        <v>20</v>
+        <v>0.29228900000000002</v>
       </c>
       <c r="AL32" s="1">
-        <v>43</v>
-      </c>
-      <c r="AM32" s="1">
-        <v>0.45260299999999998</v>
-      </c>
-      <c r="AN32" s="1">
-        <v>0.43103000000000002</v>
-      </c>
-      <c r="AO32" s="1">
-        <v>9.8665000000000003E-2</v>
-      </c>
-      <c r="AP32" s="1">
-        <v>0.29228900000000002</v>
-      </c>
-      <c r="AQ32" s="1">
         <v>0.74783699999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1">
         <v>100</v>
@@ -4775,108 +4280,93 @@
         <v>0.73564799999999997</v>
       </c>
       <c r="I33" s="1">
-        <v>0</v>
+        <v>11.443535000000001</v>
       </c>
       <c r="J33" s="1">
-        <v>0</v>
+        <v>11.133914000000001</v>
       </c>
       <c r="K33" s="1">
-        <v>0</v>
+        <v>2.9221010000000001</v>
       </c>
       <c r="L33" s="1">
-        <v>0</v>
+        <v>4.838457</v>
       </c>
       <c r="M33" s="1">
-        <v>0</v>
+        <v>19.735389999999999</v>
       </c>
       <c r="N33" s="1">
-        <v>11.443535000000001</v>
+        <v>4.4770000000000003</v>
       </c>
       <c r="O33" s="1">
-        <v>11.133914000000001</v>
+        <v>4.0529999999999999</v>
       </c>
       <c r="P33" s="1">
-        <v>2.9221010000000001</v>
+        <v>2.2681</v>
       </c>
       <c r="Q33" s="1">
-        <v>4.838457</v>
+        <v>0.28610000000000002</v>
       </c>
       <c r="R33" s="1">
-        <v>19.735389999999999</v>
+        <v>10.0282</v>
       </c>
       <c r="S33" s="1">
-        <v>4.4770000000000003</v>
+        <v>6.9440999999999997</v>
       </c>
       <c r="T33" s="1">
-        <v>4.0529999999999999</v>
+        <v>6.8982999999999999</v>
       </c>
       <c r="U33" s="1">
-        <v>2.2681</v>
+        <v>2.5446</v>
       </c>
       <c r="V33" s="1">
-        <v>0.28610000000000002</v>
+        <v>1.3002</v>
       </c>
       <c r="W33" s="1">
-        <v>10.0282</v>
+        <v>14.6645</v>
       </c>
       <c r="X33" s="1">
-        <v>6.9440999999999997</v>
+        <v>11.869</v>
       </c>
       <c r="Y33" s="1">
-        <v>6.8982999999999999</v>
+        <v>11.7971</v>
       </c>
       <c r="Z33" s="1">
-        <v>2.5446</v>
+        <v>1.6122000000000001</v>
       </c>
       <c r="AA33" s="1">
-        <v>1.3002</v>
+        <v>8.4710999999999999</v>
       </c>
       <c r="AB33" s="1">
-        <v>14.6645</v>
+        <v>16.176100000000002</v>
       </c>
       <c r="AC33" s="1">
-        <v>11.869</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="AD33" s="1">
-        <v>11.7971</v>
+        <v>33.5</v>
       </c>
       <c r="AE33" s="1">
-        <v>1.6122000000000001</v>
+        <v>5.1315999999999997</v>
       </c>
       <c r="AF33" s="1">
-        <v>8.4710999999999999</v>
+        <v>24</v>
       </c>
       <c r="AG33" s="1">
-        <v>16.176100000000002</v>
+        <v>50</v>
       </c>
       <c r="AH33" s="1">
-        <v>33.700000000000003</v>
+        <v>0.366759</v>
       </c>
       <c r="AI33" s="1">
-        <v>33.5</v>
+        <v>0.34636800000000001</v>
       </c>
       <c r="AJ33" s="1">
-        <v>5.1315999999999997</v>
+        <v>8.4071000000000007E-2</v>
       </c>
       <c r="AK33" s="1">
-        <v>24</v>
+        <v>0.218552</v>
       </c>
       <c r="AL33" s="1">
-        <v>50</v>
-      </c>
-      <c r="AM33" s="1">
-        <v>0.366759</v>
-      </c>
-      <c r="AN33" s="1">
-        <v>0.34636800000000001</v>
-      </c>
-      <c r="AO33" s="1">
-        <v>8.4071000000000007E-2</v>
-      </c>
-      <c r="AP33" s="1">
-        <v>0.218552</v>
-      </c>
-      <c r="AQ33" s="1">
         <v>0.61061699999999997</v>
       </c>
     </row>

</xml_diff>